<commit_message>
Render qmd file to generate README and update Excel file
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -365,27 +365,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>brief_description</t>
+          <t>tool_description</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>name_of_developer_maintainer_or_key_contact</t>
+          <t>contact_name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>email_of_developer_maintainer_or_key_contact</t>
+          <t>contact_email</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>is_it_actively_maintained_yes_no</t>
+          <t>is_maintained</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>relevant_disease_s</t>
+          <t>relevant_diseases</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -410,27 +410,27 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>required_expertise_to_use_tool</t>
+          <t>required_expertise</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>type_of_tool</t>
+          <t>tool_type</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>type_of_data_input_needed</t>
+          <t>input_type</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>link_to_web_page_documentation_optional</t>
+          <t>docs_link</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>link_to_source_code_optional</t>
+          <t>source_link</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -440,22 +440,22 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>github_repo_new_or_old_if_existing_one</t>
+          <t>github_link</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>complete_yes_no</t>
+          <t>is_complete</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>pkg_dev_assessment_how_hard_is_to_make_into_a_package_notes</t>
+          <t>pkg_dev_assessment</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>overall_assessment_easy_win_needs_some_work_needs_lots_of_work_long_term_project</t>
+          <t>overall_assessment</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel after merging #25
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,32 +430,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>source_link</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>reviewer</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
           <t>github_link</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>is_complete</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>pkg_dev_assessment</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>overall_assessment</t>
         </is>
       </c>
     </row>
@@ -530,16 +505,6 @@
           <t>1-Toth D, Gundlapalli A, Schell W, Bulmahn K, Walton T, Woods C, Coghill C, Gallegos F, Samore M, Adler F (2013). Quantitative models of the dose-response and time course of inhalational anthrax in humans. PLoS Pathog, 9(8), e1003555. https://doi.org/10.1371/journal.ppat.1003555.                          2-Bulmahn K, Canella M, Coghill C, Gallegos F, Gundlapalli A, Schell W, Toth D, Walton T, Woods C (2012). Final Supplementary Risk Assessment for the Boston University National Emerging Infectious Diseases Laboratories, National Institutes of Health. https://www.bu.edu/neidl/files/2013/01/SFEIR-Volume-III.pdf.</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -612,21 +577,6 @@
           <t>no pubication plan</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Nothing to do but publish analysis files.  Yue will publish those</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -699,31 +649,9 @@
           <t>https://ojs.aaai.org/index.php/AAAI/article/view/30337</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>https://github.com/Krishuthapa/SWE-Attention</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Potentially a python module. There are functions and classes that are well-defined. Maybe exporting the classes should be enough._x000D_
-_x000D_
-But it also has hardcoded stuff in the class def files.</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Needs some work - Functions/classes are mixed with the code. Need to separate them and add them to namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -796,11 +724,6 @@
       <c r="N5" t="inlineStr">
         <is>
           <t>Nothing published.</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Andrew</t>
         </is>
       </c>
     </row>
@@ -881,29 +804,9 @@
 7.Thomas A, Redd A, Khader K, Leecaster M, Greene T, Samore M (2015). Efficient parameter estimation for models of healthcare-associated pathogen transmission in discrete and continuous time. Math Med Biol, 32(1), 79-98.</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>https://github.com/EpiForeSITE/bayesian-transmission</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>A large C++ program. Probably easy to write a cmd line wrapper within R. We could also use Rcpp11.</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
         </is>
       </c>
     </row>
@@ -979,29 +882,9 @@
 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>https://github.com/EpiForeSITE/branching_process/</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>All code is functions only. It could be bundled into an R pkg very easily. We only need to have an example so it is more complete.</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1076,11 +959,6 @@
           <t>Beams A, Keegan L, Adler F, Samore M, Khader K, Toth D (2023), Are Staphylococcus aureus Carrier Types Evidence of Population Heterogeneity? American Journal of Epidemiology 192(3), 455–466. https://doi.org/10.1093/aje/kwac201.</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1153,11 +1031,6 @@
           <t>https://journals.lww.com/epidem/fulltext/2014/07000/hospital_acquired_clostridium_difficile.15.aspx</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1230,29 +1103,9 @@
           <t>https://journals.lww.com/epidem/fulltext/2022/07000/carceral_amplification_of_covid_19__impacts_for.6.aspx</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>https://github.com/epimodels/COVID19-Jails</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>It looks fairly complex, but the functions are isolated enough to be packaged out.</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1327,29 +1180,9 @@
           <t>https://www.mdpi.com/1660-4601/18/16/8260</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>https://github.com/epimodels/inperson_sports</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>No clear idea of the code structure. It has well defined functions and classes, but it mixes python and R.</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>Needs some work - Functions/classes are mixed with the code. Need to separate them and add them to namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1424,11 +1257,6 @@
           <t>Not published but will</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1501,29 +1329,9 @@
           <t>https://www.nature.com/articles/s41598-021-86811-0</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>https://github.com/HopkinsIDD/COVIDScenarioPipeline</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>It is a collection of packages building a pipeline. Already in container form, maybe could be used to build as a package.</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
         </is>
       </c>
     </row>
@@ -1598,29 +1406,9 @@
           <t>Published: https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1010352 for the canonical reference</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>https://github.com/epimodels/Metapopulation_MRSA</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Some mix of R and python code. Python functions (which run the analysis) are mostly isolated.</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>Needs some work - Functions/classes are mixed with the code. Need to separate them and add them to namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1695,11 +1483,6 @@
           <t xml:space="preserve">Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1772,11 +1555,6 @@
           <t>https://www.dediscover.org/</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1850,11 +1628,6 @@
 2-Bulmahn K, Canella M, Coghill C, Gallegos F, Gundlapalli A, Schell W, Toth D, Walton T, Woods C (2012). Final Supplementary Risk Assessment for the Boston University National Emerging Infectious Diseases Laboratories, National Institutes of Health. https://www.bu.edu/neidl/files/2013/01/SFEIR-Volume-III.pdf (Chapter 8; Appendix J).</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1927,11 +1700,6 @@
           <t>Not published but will</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2004,21 +1772,6 @@
           <t>manuscript under preparation</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>Nothing to do but publish analysis files.  Yue will publish those</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2091,21 +1844,6 @@
           <t>manuscript under preparation</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>Exists in python needs tranlation to R</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2173,14 +1911,9 @@
           <t>https://github.com/UofUEpiBio/epiworld, https://github.com/UofUEpiBio/epiworldR/, https://github.com/UofUEpiBio/epiworldpy, https://github.com/UofUEpiBio/epiworldRShiny</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t>https://github.com/UofUEpiBio/epiworld</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>yes</t>
         </is>
       </c>
     </row>
@@ -2250,7 +1983,7 @@
           <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="O22" t="inlineStr">
         <is>
           <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
@@ -2327,11 +2060,6 @@
           <t>Not currently published.</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2379,16 +2107,6 @@
           <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2451,16 +2169,6 @@
           <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2533,16 +2241,6 @@
           <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2615,16 +2313,6 @@
           <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2698,11 +2386,6 @@
 o	Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2775,16 +2458,6 @@
           <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2857,16 +2530,6 @@
           <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2940,11 +2603,6 @@
 2-Manuscript with age-structured model in preparation</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3017,16 +2675,6 @@
           <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3099,16 +2747,6 @@
           <t>https://www.nature.com/articles/s41591-021-01563-8</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3181,16 +2819,6 @@
           <t>Pending</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3263,16 +2891,6 @@
           <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3345,11 +2963,6 @@
           <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3422,31 +3035,9 @@
           <t>Preprint ready by June</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
+      <c r="O37" t="inlineStr">
         <is>
           <t>https://github.com/madhobi/multitask_unit_and_days</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>Has a handful of functions (3) well-defined. This could be a small python package._x000D_
-_x000D_
-Functions for paper figures can be set aside.</t>
-        </is>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -3521,16 +3112,6 @@
           <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="T38" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3603,11 +3184,6 @@
           <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3682,32 +3258,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
           <t>https://github.com/tdavislab/PhenoMapper</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>This extends another library, not sure if we should be putting effort here.</t>
-        </is>
-      </c>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
         </is>
       </c>
     </row>
@@ -3782,29 +3333,9 @@
           <t>Unknown</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
+      <c r="O41" t="inlineStr">
         <is>
           <t>https://github.com/kingaa/pomp</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>This package is already on CRAN. Not sure what we can do with it.</t>
-        </is>
-      </c>
-      <c r="T41" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
         </is>
       </c>
     </row>
@@ -3879,11 +3410,6 @@
           <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3956,29 +3482,9 @@
           <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
+      <c r="O43" t="inlineStr">
         <is>
           <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>The repo looks neat. I think packaging the functions should be straight forward.</t>
-        </is>
-      </c>
-      <c r="T43" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -4028,7 +3534,7 @@
           <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
         </is>
       </c>
-      <c r="Q44" t="inlineStr">
+      <c r="O44" t="inlineStr">
         <is>
           <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
@@ -4100,11 +3606,6 @@
           <t>The R code is developed, but not documented.</t>
         </is>
       </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4177,16 +3678,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4259,11 +3750,6 @@
           <t>None</t>
         </is>
       </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4336,16 +3822,6 @@
           <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4418,11 +3894,6 @@
           <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4495,11 +3966,6 @@
           <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4572,11 +4038,6 @@
           <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4649,11 +4110,6 @@
           <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4726,11 +4182,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4803,11 +4254,6 @@
           <t>https://doi.org/10.1080/17513758.2023.2298988</t>
         </is>
       </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4878,21 +4324,6 @@
       <c r="N55" t="inlineStr">
         <is>
           <t>Not published but will</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>Nothing to do but publish analysis files.  Yue will publish those</t>
-        </is>
-      </c>
-      <c r="T55" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Use concise key names in YML files (#23)
* Use concise names in YML files

* Create gitignore

* Render qmd file to generate README and update Excel file

* Make README.qmd syntax consistent

* Clean YML Files (#25)

* Remove four unneeded YML fields

* Remove source_link (deprecated) from YML files

* Update Excel after merging #25
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,27 +365,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>brief_description</t>
+          <t>tool_description</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>name_of_developer_maintainer_or_key_contact</t>
+          <t>contact_name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>email_of_developer_maintainer_or_key_contact</t>
+          <t>contact_email</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>is_it_actively_maintained_yes_no</t>
+          <t>is_maintained</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>relevant_disease_s</t>
+          <t>relevant_diseases</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -410,52 +410,27 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>required_expertise_to_use_tool</t>
+          <t>required_expertise</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>type_of_tool</t>
+          <t>tool_type</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>type_of_data_input_needed</t>
+          <t>input_type</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>link_to_web_page_documentation_optional</t>
+          <t>docs_link</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>link_to_source_code_optional</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>reviewer</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>github_repo_new_or_old_if_existing_one</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>complete_yes_no</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>pkg_dev_assessment_how_hard_is_to_make_into_a_package_notes</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>overall_assessment_easy_win_needs_some_work_needs_lots_of_work_long_term_project</t>
+          <t>github_link</t>
         </is>
       </c>
     </row>
@@ -530,16 +505,6 @@
           <t>1-Toth D, Gundlapalli A, Schell W, Bulmahn K, Walton T, Woods C, Coghill C, Gallegos F, Samore M, Adler F (2013). Quantitative models of the dose-response and time course of inhalational anthrax in humans. PLoS Pathog, 9(8), e1003555. https://doi.org/10.1371/journal.ppat.1003555.                          2-Bulmahn K, Canella M, Coghill C, Gallegos F, Gundlapalli A, Schell W, Toth D, Walton T, Woods C (2012). Final Supplementary Risk Assessment for the Boston University National Emerging Infectious Diseases Laboratories, National Institutes of Health. https://www.bu.edu/neidl/files/2013/01/SFEIR-Volume-III.pdf.</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -612,21 +577,6 @@
           <t>no pubication plan</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Nothing to do but publish analysis files.  Yue will publish those</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -699,31 +649,9 @@
           <t>https://ojs.aaai.org/index.php/AAAI/article/view/30337</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>https://github.com/Krishuthapa/SWE-Attention</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Potentially a python module. There are functions and classes that are well-defined. Maybe exporting the classes should be enough._x000D_
-_x000D_
-But it also has hardcoded stuff in the class def files.</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Needs some work - Functions/classes are mixed with the code. Need to separate them and add them to namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -796,11 +724,6 @@
       <c r="N5" t="inlineStr">
         <is>
           <t>Nothing published.</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Andrew</t>
         </is>
       </c>
     </row>
@@ -881,29 +804,9 @@
 7.Thomas A, Redd A, Khader K, Leecaster M, Greene T, Samore M (2015). Efficient parameter estimation for models of healthcare-associated pathogen transmission in discrete and continuous time. Math Med Biol, 32(1), 79-98.</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>https://github.com/EpiForeSITE/bayesian-transmission</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>A large C++ program. Probably easy to write a cmd line wrapper within R. We could also use Rcpp11.</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
         </is>
       </c>
     </row>
@@ -979,29 +882,9 @@
 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>https://github.com/EpiForeSITE/branching_process/</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>All code is functions only. It could be bundled into an R pkg very easily. We only need to have an example so it is more complete.</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1076,11 +959,6 @@
           <t>Beams A, Keegan L, Adler F, Samore M, Khader K, Toth D (2023), Are Staphylococcus aureus Carrier Types Evidence of Population Heterogeneity? American Journal of Epidemiology 192(3), 455–466. https://doi.org/10.1093/aje/kwac201.</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1153,11 +1031,6 @@
           <t>https://journals.lww.com/epidem/fulltext/2014/07000/hospital_acquired_clostridium_difficile.15.aspx</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1230,29 +1103,9 @@
           <t>https://journals.lww.com/epidem/fulltext/2022/07000/carceral_amplification_of_covid_19__impacts_for.6.aspx</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>https://github.com/epimodels/COVID19-Jails</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>It looks fairly complex, but the functions are isolated enough to be packaged out.</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1327,29 +1180,9 @@
           <t>https://www.mdpi.com/1660-4601/18/16/8260</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>https://github.com/epimodels/inperson_sports</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>No clear idea of the code structure. It has well defined functions and classes, but it mixes python and R.</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>Needs some work - Functions/classes are mixed with the code. Need to separate them and add them to namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1424,11 +1257,6 @@
           <t>Not published but will</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1501,29 +1329,9 @@
           <t>https://www.nature.com/articles/s41598-021-86811-0</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>https://github.com/HopkinsIDD/COVIDScenarioPipeline</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>It is a collection of packages building a pipeline. Already in container form, maybe could be used to build as a package.</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
         </is>
       </c>
     </row>
@@ -1598,29 +1406,9 @@
           <t>Published: https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1010352 for the canonical reference</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>https://github.com/epimodels/Metapopulation_MRSA</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Some mix of R and python code. Python functions (which run the analysis) are mostly isolated.</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>Needs some work - Functions/classes are mixed with the code. Need to separate them and add them to namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -1695,11 +1483,6 @@
           <t xml:space="preserve">Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1772,11 +1555,6 @@
           <t>https://www.dediscover.org/</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1850,11 +1628,6 @@
 2-Bulmahn K, Canella M, Coghill C, Gallegos F, Gundlapalli A, Schell W, Toth D, Walton T, Woods C (2012). Final Supplementary Risk Assessment for the Boston University National Emerging Infectious Diseases Laboratories, National Institutes of Health. https://www.bu.edu/neidl/files/2013/01/SFEIR-Volume-III.pdf (Chapter 8; Appendix J).</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1927,11 +1700,6 @@
           <t>Not published but will</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2004,21 +1772,6 @@
           <t>manuscript under preparation</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>Nothing to do but publish analysis files.  Yue will publish those</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2091,21 +1844,6 @@
           <t>manuscript under preparation</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>Exists in python needs tranlation to R</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2173,14 +1911,9 @@
           <t>https://github.com/UofUEpiBio/epiworld, https://github.com/UofUEpiBio/epiworldR/, https://github.com/UofUEpiBio/epiworldpy, https://github.com/UofUEpiBio/epiworldRShiny</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t>https://github.com/UofUEpiBio/epiworld</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>yes</t>
         </is>
       </c>
     </row>
@@ -2250,7 +1983,7 @@
           <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="O22" t="inlineStr">
         <is>
           <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
@@ -2327,11 +2060,6 @@
           <t>Not currently published.</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2379,16 +2107,6 @@
           <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2451,16 +2169,6 @@
           <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2533,16 +2241,6 @@
           <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2615,16 +2313,6 @@
           <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2698,11 +2386,6 @@
 o	Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2775,16 +2458,6 @@
           <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2857,16 +2530,6 @@
           <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2940,11 +2603,6 @@
 2-Manuscript with age-structured model in preparation</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3017,16 +2675,6 @@
           <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3099,16 +2747,6 @@
           <t>https://www.nature.com/articles/s41591-021-01563-8</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3181,16 +2819,6 @@
           <t>Pending</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3263,16 +2891,6 @@
           <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3345,11 +2963,6 @@
           <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3422,31 +3035,9 @@
           <t>Preprint ready by June</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
+      <c r="O37" t="inlineStr">
         <is>
           <t>https://github.com/madhobi/multitask_unit_and_days</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>Has a handful of functions (3) well-defined. This could be a small python package._x000D_
-_x000D_
-Functions for paper figures can be set aside.</t>
-        </is>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -3521,16 +3112,6 @@
           <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="T38" t="inlineStr">
-        <is>
-          <t>Leave for later - Too complex to address | No functional programming whatsoever</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3603,11 +3184,6 @@
           <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3682,32 +3258,7 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
           <t>https://github.com/tdavislab/PhenoMapper</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>This extends another library, not sure if we should be putting effort here.</t>
-        </is>
-      </c>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
         </is>
       </c>
     </row>
@@ -3782,29 +3333,9 @@
           <t>Unknown</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
+      <c r="O41" t="inlineStr">
         <is>
           <t>https://github.com/kingaa/pomp</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>This package is already on CRAN. Not sure what we can do with it.</t>
-        </is>
-      </c>
-      <c r="T41" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
         </is>
       </c>
     </row>
@@ -3879,11 +3410,6 @@
           <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3956,29 +3482,9 @@
           <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
+      <c r="O43" t="inlineStr">
         <is>
           <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>The repo looks neat. I think packaging the functions should be straight forward.</t>
-        </is>
-      </c>
-      <c r="T43" t="inlineStr">
-        <is>
-          <t>Easy win - Functions are already in a separate file, just need to be added to a namespace/__init__.py file.</t>
         </is>
       </c>
     </row>
@@ -4028,7 +3534,7 @@
           <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
         </is>
       </c>
-      <c r="Q44" t="inlineStr">
+      <c r="O44" t="inlineStr">
         <is>
           <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
@@ -4100,11 +3606,6 @@
           <t>The R code is developed, but not documented.</t>
         </is>
       </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4177,16 +3678,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4259,11 +3750,6 @@
           <t>None</t>
         </is>
       </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4336,16 +3822,6 @@
           <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>Asked for the code</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4418,11 +3894,6 @@
           <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4495,11 +3966,6 @@
           <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4572,11 +4038,6 @@
           <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4649,11 +4110,6 @@
           <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4726,11 +4182,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4803,11 +4254,6 @@
           <t>https://doi.org/10.1080/17513758.2023.2298988</t>
         </is>
       </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>George</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4878,21 +4324,6 @@
       <c r="N55" t="inlineStr">
         <is>
           <t>Not published but will</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>Andrew</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>Nothing to do but publish analysis files.  Yue will publish those</t>
-        </is>
-      </c>
-      <c r="T55" t="inlineStr">
-        <is>
-          <t>Unsure - Needs group thinking</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating readme and list
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -785,7 +785,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>We’ve used Mortality Mapping (mMAP), an existing epidemiologic and statistical analysis approach by Lu et al. [1,2] to estimate the cumulative incidence of symptomatic COVID-19 in Veterans in the United States. mMAP is a time series deconvolution method which infers the true COVID-19 case counts from reported COVID-19 deaths. It uses symptom onset to death distribution, smoothed time series of reported COVID-19 deaths, and symptomatic case fatality rate (sCFR) to estimate the distribution of symptomatic COVID-19 cases. We focus on the adjusted version of the mMAP approach presented by Lu et al., which tries to account for the unreported COVID-19 deaths. While Lu uses excess influenza and pneumonia deaths to account for unreported COVID-19 deaths, we have extended their approach by using excess all-cause deaths. </t>
+          <t xml:space="preserve">We’ve used Mortality Mapping (mMAP), an existing epidemiologic and statistical analysis approach by Lu et al. [1,2] to estimate the cumulative incidence of symptomatic COVID-19 in Veterans in the United States. mMAP is a time series deconvolution method which infers the true COVID-19 case counts from reported COVID-19 deaths. It uses symptom onset to death distribution, smoothed time series of reported COVID-19 deaths, and symptomatic case fatality rate (sCFR) to estimate the distribution of symptomatic COVID-19 cases. We focus on the adjusted version of the mMAP approach presented by Lu et al., which tries to account for the unreported COVID-19 deaths. While Lu uses excess influenza and pneumonia deaths to account for unreported COVID-19 deaths, we have extended their approach by using excess all-cause deaths. </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
+          <t xml:space="preserve">Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2372,7 +2372,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -2950,7 +2950,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -4097,7 +4097,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Damon Togh</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">

</xml_diff>

<commit_message>
Add vax equity yaml, render readme. (#31)
* added vaccine_equity.yml

* render readme

* Apply suggestions from code review

* Updating readme and list

---------

Co-authored-by: George G. Vega Yon <g.vegayon@gmail.com>
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4186,52 +4186,47 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Vaccine Equity</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>An emerging infectious disease</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4246,82 +4241,159 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B56" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F56" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G56" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr">
+      <c r="M56" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N55" t="inlineStr">
+      <c r="N56" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Add YML for epiworld-forecasts, add quarto render command to data README
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1920,22 +1920,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>epiworldpy: A python wrapper for epiworld</t>
+          <t>epiworld-forecasts: Automatic Disease Forecasting with epiworldR</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
+          <t>epiworld-forecasts uses epiworldR, GitHub Actions, and Docker to generate disease forecasts that update automatically. While we provide an example forecast of COVID-19 case counts in Utah, this tool is an open-source, template repository that can easily be adapted to generate forecasts for different diseases.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>George G. Vega Yon, Milo Banks</t>
+          <t>Andrew Pulsipher</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>george.vegayon@utah.edu</t>
+          <t>a.pulsipher@utah.edu</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Alpha/Beta phase: ready for inital user testing but requires additional development and testing</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1955,12 +1955,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Forecasters</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1970,44 +1970,44 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Automation pipeline tools</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>Data sources, model definition, calibration steps</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+          <t>https://github.com/EpiForeSITE/epiworld-forecasts, https://epiforesite.github.io/epiworld-forecasts/, https://github.com/UofUEpiBio/epiworldR/</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+          <t>https://github.com/EpiForeSITE/epiworld-forecasts</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Excess Death Estimation</t>
+          <t>epiworldpy: A python wrapper for epiworld</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The aberration detection methods introduced by Farrington et al. and later Noufaily et al. have been implemented to obtain weekly all-cause mortality data.</t>
+          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Vanessa Stevens or Wathsala Widanagamaachchi</t>
+          <t>George G. Vega Yon, Milo Banks</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>vanessa.stevens@hsc.utah.edu; vanessa.stevens@va.gov or wathsala.widanagamaachchi@hsc.utah.edu</t>
+          <t>george.vegayon@utah.edu</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2015,29 +2015,24 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>None.  Kelly believes this was all cause mortality estimation.</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>We already have a version of this in operations</t>
+          <t>Alpha/Beta phase: ready for inital user testing but requires additional development and testing</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2047,39 +2042,44 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Statistical Model - Forecasting</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Data sources for this include both inpatient and outpatient mortality records. The ‘surveillance’ package in R was used to implement both the original Farrington method and the Flexible Farrington method by Noufaily et al. depending on the options specified. Control slots are used to specify which options are to be used. These options are customizable, but a strength of Farrington-based algorithms is that they are relatively robust across applications. Many of the options we have used are based on algorithm defaults. Additionally, ‘Nobbs’ nowcasting package in R was used to address delays in death reporting before applying Flexible Farrington.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Not currently published.</t>
+          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GeoCovid</t>
+          <t>Excess Death Estimation</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Shiny App for visualizing mobility data and COVID-19 cases in Buenos Aires province during March to December 2020.</t>
+          <t>The aberration detection methods introduced by Farrington et al. and later Noufaily et al. have been implemented to obtain weekly all-cause mortality data.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Maria del Pilar Fernandez</t>
+          <t>Vanessa Stevens or Wathsala Widanagamaachchi</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>pilar.fernandez@wsu.edu</t>
+          <t>vanessa.stevens@hsc.utah.edu; vanessa.stevens@va.gov or wathsala.widanagamaachchi@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2087,9 +2087,19 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>None.  Kelly believes this was all cause mortality estimation.</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Under development</t>
+          <t>We already have a version of this in operations</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2097,36 +2107,51 @@
           <t>R</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Statistical Model - Forecasting</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Data sources for this include both inpatient and outpatient mortality records. The ‘surveillance’ package in R was used to implement both the original Farrington method and the Flexible Farrington method by Noufaily et al. depending on the options specified. Control slots are used to specify which options are to be used. These options are customizable, but a strength of Farrington-based algorithms is that they are relatively robust across applications. Many of the options we have used are based on algorithm defaults. Additionally, ‘Nobbs’ nowcasting package in R was used to address delays in death reporting before applying Flexible Farrington.</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app, https://github.com/Fernandez-Lab-WSU/geocovid_bsas, https://fernandez-lab-wsu.github.io/geocovid-slides/slides.html#/geocovidar</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
+          <t>Not currently published.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Granular Modeling Framework/ICU</t>
+          <t>GeoCovid</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Implement 2 ICUs that match the CVICU at the University of Utah and the ICU at the Salt Lake City VA.  Model all empirical data collected by the GM project:  HCW movement and touch data as collected by the proximity sensors, Patient flow from the EHR, and micro data as sampled by the GM micro team.  Scenarios(s) Modeled: Sustained endemic HAI levels driven by importation into a 15-25 bed ICU.  Contamination and transmission via HCW movement and contact behaviors.  The simulation includes contamination of multiple surfaces in several room zones, contamination of patient surfaces via shedding and HCW surfaces via touching.  Room cleaning, isolation, and targeted treatment of HAI.  HCW visits include assigned networks between health care workers and patients as well as ad hoc visits.</t>
+          <t>Shiny App for visualizing mobility data and COVID-19 cases in Buenos Aires province during March to December 2020.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Willy Ray</t>
+          <t>Maria del Pilar Fernandez</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>william.ray@hcs.utah.edu</t>
+          <t>pilar.fernandez@wsu.edu</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2134,76 +2159,61 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Only C.Diff currently implemented, but all organisms sampled in the GM project were targeted.</t>
-        </is>
-      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>The framework is developed in Java/Groovy in the Repast Simphony toolset.  It is intended to be useable to quickly model fresh scenarios relatively quickly.  In practice, it is currently only useable by Willy.  Willy is able to use it to develop new models and features in existing models fairly quickly, but no-one else will be able to do that at this point.  The GM model and the underlying framework are hosted on github, but updates on the remote are far behind the commits that have been made by the developer.  The GM model itself if hung up on parameter estimation.</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Under development</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Java/Groovy</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app, https://github.com/Fernandez-Lab-WSU/geocovid_bsas, https://fernandez-lab-wsu.github.io/geocovid-slides/slides.html#/geocovidar</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>H1N1 Pandemic Data Estimation</t>
+          <t>Granular Modeling Framework/ICU</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Describes an SIR model parameter estimation with an improved fit using least squares estimation over maximum likelihood estimation. Parameter estimated: Transmission rate, recovery rate, R0, number of initial infectives</t>
+          <t>Implement 2 ICUs that match the CVICU at the University of Utah and the ICU at the Salt Lake City VA.  Model all empirical data collected by the GM project:  HCW movement and touch data as collected by the proximity sensors, Patient flow from the EHR, and micro data as sampled by the GM micro team.  Scenarios(s) Modeled: Sustained endemic HAI levels driven by importation into a 15-25 bed ICU.  Contamination and transmission via HCW movement and contact behaviors.  The simulation includes contamination of multiple surfaces in several room zones, contamination of patient surfaces via shedding and HCW surfaces via touching.  Room cleaning, isolation, and targeted treatment of HAI.  HCW visits include assigned networks between health care workers and patients as well as ad hoc visits.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Willy Ray</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>william.ray@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>N/A (basic SIR)</t>
+          <t>Only C.Diff currently implemented, but all organisms sampled in the GM project were targeted.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>N/A (LSE, MLE)</t>
+          <t>The framework is developed in Java/Groovy in the Repast Simphony toolset.  It is intended to be useable to quickly model fresh scenarios relatively quickly.  In practice, it is currently only useable by Willy.  Willy is able to use it to develop new models and features in existing models fairly quickly, but no-one else will be able to do that at this point.  The GM model and the underlying framework are hosted on github, but updates on the remote are far behind the commits that have been made by the developer.  The GM model itself if hung up on parameter estimation.</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2213,7 +2223,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Java/Groovy</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2228,39 +2238,29 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>2009 H1N1 Influenza (Swine Flu) fit to Washington State University Student Health Center data set</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Healthcare facility network outbreak simulator</t>
+          <t>H1N1 Pandemic Data Estimation</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Provides flexible framework for agent-based simulation of outbreaks among in-patients in a generic-but-realistic network of short/long-stay hospitals and nursing homes, as well as interventions to mitigate transmission and inter-facility spread. Scenarios(s) Modeled:  Initial invasion of new pathogen / strain and/or endemic pathogens. Intervention scenarios for patient-targeted efforts including surveillance and isolation (contact precautions), vaccination, and anti-microbial drug treatment.</t>
+          <t>Describes an SIR model parameter estimation with an improved fit using least squares estimation over maximum likelihood estimation. Parameter estimated: Transmission rate, recovery rate, R0, number of initial infectives</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2270,12 +2270,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen(s); we have applied the model to carbapenem-resistant Enterobacteriaceae, C. difficile, and MRSA.</t>
+          <t>N/A (basic SIR)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Effort was made to convert the model to publicly available software Repast (by Willy Ray) but was not completed.</t>
+          <t>N/A (LSE, MLE)</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2300,174 +2300,174 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Local network of hospitals and nursing homes that directly exchange patients, as well as generic “community” component to track discharged / readmitted patients after and between hospital stays.</t>
+          <t>2009 H1N1 Influenza (Swine Flu) fit to Washington State University Student Health Center data set</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
+          <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Healthcare facility network outbreak simulator</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Provides flexible framework for agent-based simulation of outbreaks among in-patients in a generic-but-realistic network of short/long-stay hospitals and nursing homes, as well as interventions to mitigate transmission and inter-facility spread. Scenarios(s) Modeled:  Initial invasion of new pathogen / strain and/or endemic pathogens. Intervention scenarios for patient-targeted efforts including surveillance and isolation (contact precautions), vaccination, and anti-microbial drug treatment.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Damon Toth</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Damon.Toth@hsc.utah.edu</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Any healthcare-associated pathogen(s); we have applied the model to carbapenem-resistant Enterobacteriaceae, C. difficile, and MRSA.</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Effort was made to convert the model to publicly available software Repast (by Willy Ray) but was not completed.</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Anylogic</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Local network of hospitals and nursing homes that directly exchange patients, as well as generic “community” component to track discharged / readmitted patients after and between hospital stays.</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>Healthcare transmission epidemiology estimation at equilibrium</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Estimate the extent of patient-to-patient transmission and other quantities using admission prevalence and cross-sectional point-prevalence data for carriage of organisms among healthcare facility in-patients. Parameter estimated: Patient-to-patient transmission rate, facility reproduction number, rate of progression to infection, intervention effects if applicable. Estimates derived via solving differential equations at equilibrium and facility reproduction number equations.</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Damon Toth</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Any healthcare-transmissible pathogen with appropriate data; we have applied our tools to carbapenem-resistant Enterobacteriaceae, C. difficile, and S. aureus.</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort. Creating an R package for facility reproduction number calculations has been discussed.</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="M29" t="inlineStr">
         <is>
           <t>Appropriate for application to data sets for patient carriage prevalence at admission and cross-sectional in-patient prevalence, when these quantities are stable over time. Contextual data for length of stay, invasive infection rates, carriage duration and intervention efforts add utility. Useful for understanding transmission risk and threshold effects in healthcare facilities, and for estimating intervention effectiveness.</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>o	Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557._x000D_
 o	Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Herpes Vaccine Model</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>An ODE-based 6-compartment SI model with asymptomatic carriers and vaccinated classes to forecast the number of infections prevented with imperfect vaccination and infections prevented per vaccine administered. Parameter estimated: Highly correlated parameters determined using LHS PRCC. Scenarios(s) Modeled: Prophylactic (pre-exposure) vaccines, Therapeutic (post-exposure) vaccines, Parameter(s) Estimated: Highly correlated parameters determined using LHS PRCC</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Elissa Schwartz</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>ejs@wsu.edu</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>HSV-2 (Herpes Simplex Virus)</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Matlab program for uncertainty and sensitivity analysis (Latin Hypercube Sampling and Partial Rank Correlation Coefficient analysis) in development and nearing completion. Old C/C++ code is being recoded in Matlab and R and should be ready soon (~April 2024).</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Matlab</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling &amp; Parameter estimation</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>Low prevalence populations (general pop), high-risk populations (high prevalence pops)</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
-        </is>
-      </c>
-    </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HIV End Stage Kidney Disease Epidemic Model</t>
+          <t>Herpes Vaccine Model</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>An ODE-based model to predict future disease prevalence given the impact of drug therapy levels and its mechanism of action (i.e., stopping progression to disease or reducing deaths). Parameter estimated:  Growth rate, death rate, drug efficacy to block disease progression. Scenarios(s) Modeled: Rebound in prevalence due to insufficient therapy (e.g., like in Paxlovid rebound).</t>
+          <t>An ODE-based 6-compartment SI model with asymptomatic carriers and vaccinated classes to forecast the number of infections prevented with imperfect vaccination and infections prevented per vaccine administered. Parameter estimated: Highly correlated parameters determined using LHS PRCC. Scenarios(s) Modeled: Prophylactic (pre-exposure) vaccines, Therapeutic (post-exposure) vaccines, Parameter(s) Estimated: Highly correlated parameters determined using LHS PRCC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2482,17 +2482,17 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>End stage kidney disease among HIV-infected population</t>
+          <t>HSV-2 (Herpes Simplex Virus)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Coded in Matlab, Berkeley Madonna, or Excel. Very easy to code up and use.</t>
+          <t>Matlab program for uncertainty and sensitivity analysis (Latin Hypercube Sampling and Partial Rank Correlation Coefficient analysis) in development and nearing completion. Old C/C++ code is being recoded in Matlab and R and should be ready soon (~April 2024).</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Coded in Matlab, Berkeley Madonna, or Excel.</t>
+          <t>Matlab</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2522,179 +2522,179 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Progression to the severe disease state, after infection. For parameter estimation: Fitting exponential growth curves to data, using Excel</t>
+          <t>Low prevalence populations (general pop), high-risk populations (high prevalence pops)</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
+          <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>HIV End Stage Kidney Disease Epidemic Model</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>An ODE-based model to predict future disease prevalence given the impact of drug therapy levels and its mechanism of action (i.e., stopping progression to disease or reducing deaths). Parameter estimated:  Growth rate, death rate, drug efficacy to block disease progression. Scenarios(s) Modeled: Rebound in prevalence due to insufficient therapy (e.g., like in Paxlovid rebound).</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>End stage kidney disease among HIV-infected population</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Coded in Matlab, Berkeley Madonna, or Excel. Very easy to code up and use.</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Coded in Matlab, Berkeley Madonna, or Excel.</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling &amp; Parameter estimation</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Progression to the severe disease state, after infection. For parameter estimation: Fitting exponential growth curves to data, using Excel</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>Household epidemiology estimation from antibody data</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>Simultaneously estimate household importation risk, household secondary attack rate, and associated variability / heterogeneities using point-prevalence data for antibody positivity among household members. Parameter estimated: Household importation probability, household secondary attack rate, sensitivity / specificity of data for indicating prior infection, variability (dispersion) in transmissibility,  and heterogeneities in those quantities over age and/or other identifiable characteristics of individuals and households. Estimates derived via maximum likelihood for final household outbreak size equations.</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>Damon Toth</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>Any household-transmissible pathogen with appropriate data; we have applied our tools to SARS-CoV-2.</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>Published</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
         <is>
           <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
-      <c r="M31" t="inlineStr">
+      <c r="M32" t="inlineStr">
         <is>
           <t>Appropriate for application to data sets for prevalence of antibody positivity (e.g. via testing of serological samples) from members of randomly sampled households; useful for understanding transmission risk in close-contact indoor settings and mechanisms of epidemiological differences across demographic factors. Can also be applied to residents/staff of small nursing homes.</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097._x000D_
 2-Manuscript with age-structured model in preparation</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Household transmission simulator</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Simulate household importation and within-household transmission across a population of households, and intervention effects, e.g. vaccination. Scenarios(s) Modeled: Household importation and transmission with variability in transmissibility and heterogeneity across age groups and vaccination status.</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Damon Toth</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Any household-transmissible pathogen; tool has previously been used for SARS-CoV-2</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>R code for basic simulation is publicly available [https://github.com/damontoth/householdTransmission]. Extensions with age heterogeneity and vaccination are under development. Could be packaged for wider use.</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>A population of households in a given area; previously applied to a distribution of households representative of Utah. Can also be applied to residents / staff of small nursing homes.</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
-        </is>
-      </c>
-    </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Impact of school opening model on SARS-CoV-2 community incidence and mortality</t>
+          <t>Household transmission simulator</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The goal of this statistical analysis was to compare SARS-CoV-2 community incidence and mortality rates across schools that opened in in-person, remote, or hybrid mode. Measure(s) of Economic Impact: Infections and mortality</t>
+          <t>Simulate household importation and within-household transmission across a population of households, and intervention effects, e.g. vaccination. Scenarios(s) Modeled: Household importation and transmission with variability in transmissibility and heterogeneity across age groups and vaccination status.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2704,12 +2704,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Any household-transmissible pathogen; tool has previously been used for SARS-CoV-2</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>The Stata code for this analysis was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>R code for basic simulation is publicly available [https://github.com/damontoth/householdTransmission]. Extensions with age heterogeneity and vaccination are under development. Could be packaged for wider use.</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2734,39 +2734,39 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Statistical Model - Forecasting</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>The statistical model was developed using data on school mode from Burbio, SARS-CoV-2 and mortality rates from CDC, and mobility data from Google.</t>
+          <t>A population of households in a given area; previously applied to a distribution of households representative of Utah. Can also be applied to residents / staff of small nursing homes.</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>https://www.nature.com/articles/s41591-021-01563-8</t>
+          <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Inpatient antibiotic prescribing and effects simulator</t>
+          <t>Impact of school opening model on SARS-CoV-2 community incidence and mortality</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Simulate realistic rates and timing / duration / types of antibiotic administration to hospital inpatients and their effects on microbial transmission and infection, and antibiotic stewardship effects. Scenarios(s) Modeled:  Prescribing patterns of different types of antibiotics based on U.S. data; intervention scenarios for reducing prescribing, shortening duration of courses, and altering types of antibiotics used.</t>
+          <t>The goal of this statistical analysis was to compare SARS-CoV-2 community incidence and mortality rates across schools that opened in in-person, remote, or hybrid mode. Measure(s) of Economic Impact: Infections and mortality</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2776,12 +2776,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Any pathogen with supportable assumptions for antibiotic effects on hospital epidemiology; we have applied our tools to C. difficile.</t>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>R code is organized and documented but not publicly available. Could be made publicly available or packaged for use with moderate effort.</t>
+          <t>The Stata code for this analysis was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2806,29 +2806,29 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Statistical Model - Forecasting</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Single facility or small network of facilities</t>
+          <t>The statistical model was developed using data on school mode from Burbio, SARS-CoV-2 and mortality rates from CDC, and mobility data from Google.</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>https://www.nature.com/articles/s41591-021-01563-8</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Long-term acute care hospital (LTACH) intervention model</t>
+          <t>Inpatient antibiotic prescribing and effects simulator</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
+          <t>Simulate realistic rates and timing / duration / types of antibiotic administration to hospital inpatients and their effects on microbial transmission and infection, and antibiotic stewardship effects. Scenarios(s) Modeled:  Prescribing patterns of different types of antibiotics based on U.S. data; intervention scenarios for reducing prescribing, shortening duration of courses, and altering types of antibiotics used.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2848,12 +2848,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
+          <t>Any pathogen with supportable assumptions for antibiotic effects on hospital epidemiology; we have applied our tools to C. difficile.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>R code is organized and documented but not publicly available. Could be made publicly available or packaged for use with moderate effort.</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2883,49 +2883,49 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
+          <t>Single facility or small network of facilities</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Monolix</t>
+          <t>Long-term acute care hospital (LTACH) intervention model</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
+          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2935,12 +2935,12 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2950,39 +2950,39 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>https://monolix.lixoft.com/</t>
+          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Monolix</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2992,12 +2992,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Any hospital admission</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3007,12 +3007,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3022,59 +3022,54 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3084,7 +3079,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -3104,49 +3099,54 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3171,54 +3171,54 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,59 +3243,54 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3305,7 +3300,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3325,54 +3320,54 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3397,39 +3392,44 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3439,12 +3439,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3469,59 +3469,69 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3529,66 +3539,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3596,36 +3601,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -3635,12 +3640,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3650,7 +3655,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3665,39 +3670,34 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3742,24 +3742,24 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3779,12 +3779,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3814,34 +3814,34 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3851,12 +3851,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3881,54 +3881,54 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3953,54 +3953,54 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4025,39 +4025,39 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -4067,12 +4067,12 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4102,34 +4102,34 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4139,12 +4139,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -4169,64 +4169,69 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4241,69 +4246,59 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Vaccine Equity</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>An emerging infectious disease</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4318,82 +4313,159 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G57" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr">
+      <c r="M57" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N56" t="inlineStr">
+      <c r="N57" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Automatically build README file from quarto (#41)
* Add YML for epiworld-forecasts, add quarto render command to data README

* Initial draft of workflow for automatically building README

* Add path to README.qmd in GHA

* Update GHA to use tidyverse container

* Add install dependencies to GHA

* Update quarto-build-readme.yml

* Update quarto-build-readme.yml

* Update quarto-build-readme.yml

* Update quarto-build-readme.yml

* Automatic README update

* Clean up workflow file

* Automatic README update

* Only run README build workflow if data/ or .qmd files change

* Check only for changes to yml files in data/

* Automatic README update

* Automatic README update

* Automatic README update
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -785,7 +785,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">We’ve used Mortality Mapping (mMAP), an existing epidemiologic and statistical analysis approach by Lu et al. [1,2] to estimate the cumulative incidence of symptomatic COVID-19 in Veterans in the United States. mMAP is a time series deconvolution method which infers the true COVID-19 case counts from reported COVID-19 deaths. It uses symptom onset to death distribution, smoothed time series of reported COVID-19 deaths, and symptomatic case fatality rate (sCFR) to estimate the distribution of symptomatic COVID-19 cases. We focus on the adjusted version of the mMAP approach presented by Lu et al., which tries to account for the unreported COVID-19 deaths. While Lu uses excess influenza and pneumonia deaths to account for unreported COVID-19 deaths, we have extended their approach by using excess all-cause deaths. </t>
+          <t>We’ve used Mortality Mapping (mMAP), an existing epidemiologic and statistical analysis approach by Lu et al. [1,2] to estimate the cumulative incidence of symptomatic COVID-19 in Veterans in the United States. mMAP is a time series deconvolution method which infers the true COVID-19 case counts from reported COVID-19 deaths. It uses symptom onset to death distribution, smoothed time series of reported COVID-19 deaths, and symptomatic case fatality rate (sCFR) to estimate the distribution of symptomatic COVID-19 cases. We focus on the adjusted version of the mMAP approach presented by Lu et al., which tries to account for the unreported COVID-19 deaths. While Lu uses excess influenza and pneumonia deaths to account for unreported COVID-19 deaths, we have extended their approach by using excess all-cause deaths. </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
+          <t>Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1920,22 +1920,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>epiworldpy: A python wrapper for epiworld</t>
+          <t>epiworld-forecasts: Automatic Disease Forecasting with epiworldR</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
+          <t>epiworld-forecasts uses epiworldR, GitHub Actions, and Docker to generate disease forecasts that update automatically. While we provide an example forecast of COVID-19 case counts in Utah, this tool is an open-source, template repository that can easily be adapted to generate forecasts for different diseases.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>George G. Vega Yon, Milo Banks</t>
+          <t>Andrew Pulsipher</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>george.vegayon@utah.edu</t>
+          <t>a.pulsipher@utah.edu</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Alpha/Beta phase: ready for inital user testing but requires additional development and testing</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1955,12 +1955,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Forecasters</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1970,44 +1970,44 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Automation pipeline tool</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>Data sources, model definition, calibration steps</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+          <t>https://github.com/EpiForeSITE/epiworld-forecasts, https://epiforesite.github.io/epiworld-forecasts/, https://github.com/UofUEpiBio/epiworldR/</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+          <t>https://github.com/EpiForeSITE/epiworld-forecasts</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Excess Death Estimation</t>
+          <t>epiworldpy: A python wrapper for epiworld</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The aberration detection methods introduced by Farrington et al. and later Noufaily et al. have been implemented to obtain weekly all-cause mortality data.</t>
+          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Vanessa Stevens or Wathsala Widanagamaachchi</t>
+          <t>George G. Vega Yon, Milo Banks</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>vanessa.stevens@hsc.utah.edu; vanessa.stevens@va.gov or wathsala.widanagamaachchi@hsc.utah.edu</t>
+          <t>george.vegayon@utah.edu</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2015,29 +2015,24 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>None.  Kelly believes this was all cause mortality estimation.</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>We already have a version of this in operations</t>
+          <t>Alpha/Beta phase: ready for inital user testing but requires additional development and testing</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2047,39 +2042,44 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Statistical Model - Forecasting</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Data sources for this include both inpatient and outpatient mortality records. The ‘surveillance’ package in R was used to implement both the original Farrington method and the Flexible Farrington method by Noufaily et al. depending on the options specified. Control slots are used to specify which options are to be used. These options are customizable, but a strength of Farrington-based algorithms is that they are relatively robust across applications. Many of the options we have used are based on algorithm defaults. Additionally, ‘Nobbs’ nowcasting package in R was used to address delays in death reporting before applying Flexible Farrington.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Not currently published.</t>
+          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GeoCovid</t>
+          <t>Excess Death Estimation</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Shiny App for visualizing mobility data and COVID-19 cases in Buenos Aires province during March to December 2020.</t>
+          <t>The aberration detection methods introduced by Farrington et al. and later Noufaily et al. have been implemented to obtain weekly all-cause mortality data.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Maria del Pilar Fernandez</t>
+          <t>Vanessa Stevens or Wathsala Widanagamaachchi</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>pilar.fernandez@wsu.edu</t>
+          <t>vanessa.stevens@hsc.utah.edu; vanessa.stevens@va.gov or wathsala.widanagamaachchi@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2087,9 +2087,19 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>None.  Kelly believes this was all cause mortality estimation.</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Under development</t>
+          <t>We already have a version of this in operations</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2097,36 +2107,51 @@
           <t>R</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Statistical Model - Forecasting</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Data sources for this include both inpatient and outpatient mortality records. The ‘surveillance’ package in R was used to implement both the original Farrington method and the Flexible Farrington method by Noufaily et al. depending on the options specified. Control slots are used to specify which options are to be used. These options are customizable, but a strength of Farrington-based algorithms is that they are relatively robust across applications. Many of the options we have used are based on algorithm defaults. Additionally, ‘Nobbs’ nowcasting package in R was used to address delays in death reporting before applying Flexible Farrington.</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app, https://github.com/Fernandez-Lab-WSU/geocovid_bsas, https://fernandez-lab-wsu.github.io/geocovid-slides/slides.html#/geocovidar</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
+          <t>Not currently published.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Granular Modeling Framework/ICU</t>
+          <t>GeoCovid</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Implement 2 ICUs that match the CVICU at the University of Utah and the ICU at the Salt Lake City VA.  Model all empirical data collected by the GM project:  HCW movement and touch data as collected by the proximity sensors, Patient flow from the EHR, and micro data as sampled by the GM micro team.  Scenarios(s) Modeled: Sustained endemic HAI levels driven by importation into a 15-25 bed ICU.  Contamination and transmission via HCW movement and contact behaviors.  The simulation includes contamination of multiple surfaces in several room zones, contamination of patient surfaces via shedding and HCW surfaces via touching.  Room cleaning, isolation, and targeted treatment of HAI.  HCW visits include assigned networks between health care workers and patients as well as ad hoc visits.</t>
+          <t>Shiny App for visualizing mobility data and COVID-19 cases in Buenos Aires province during March to December 2020.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Willy Ray</t>
+          <t>Maria del Pilar Fernandez</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>william.ray@hcs.utah.edu</t>
+          <t>pilar.fernandez@wsu.edu</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2134,76 +2159,61 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Only C.Diff currently implemented, but all organisms sampled in the GM project were targeted.</t>
-        </is>
-      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>The framework is developed in Java/Groovy in the Repast Simphony toolset.  It is intended to be useable to quickly model fresh scenarios relatively quickly.  In practice, it is currently only useable by Willy.  Willy is able to use it to develop new models and features in existing models fairly quickly, but no-one else will be able to do that at this point.  The GM model and the underlying framework are hosted on github, but updates on the remote are far behind the commits that have been made by the developer.  The GM model itself if hung up on parameter estimation.</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Under development</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Java/Groovy</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app, https://github.com/Fernandez-Lab-WSU/geocovid_bsas, https://fernandez-lab-wsu.github.io/geocovid-slides/slides.html#/geocovidar</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>H1N1 Pandemic Data Estimation</t>
+          <t>Granular Modeling Framework/ICU</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Describes an SIR model parameter estimation with an improved fit using least squares estimation over maximum likelihood estimation. Parameter estimated: Transmission rate, recovery rate, R0, number of initial infectives</t>
+          <t>Implement 2 ICUs that match the CVICU at the University of Utah and the ICU at the Salt Lake City VA.  Model all empirical data collected by the GM project:  HCW movement and touch data as collected by the proximity sensors, Patient flow from the EHR, and micro data as sampled by the GM micro team.  Scenarios(s) Modeled: Sustained endemic HAI levels driven by importation into a 15-25 bed ICU.  Contamination and transmission via HCW movement and contact behaviors.  The simulation includes contamination of multiple surfaces in several room zones, contamination of patient surfaces via shedding and HCW surfaces via touching.  Room cleaning, isolation, and targeted treatment of HAI.  HCW visits include assigned networks between health care workers and patients as well as ad hoc visits.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Willy Ray</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>william.ray@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>N/A (basic SIR)</t>
+          <t>Only C.Diff currently implemented, but all organisms sampled in the GM project were targeted.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>N/A (LSE, MLE)</t>
+          <t>The framework is developed in Java/Groovy in the Repast Simphony toolset.  It is intended to be useable to quickly model fresh scenarios relatively quickly.  In practice, it is currently only useable by Willy.  Willy is able to use it to develop new models and features in existing models fairly quickly, but no-one else will be able to do that at this point.  The GM model and the underlying framework are hosted on github, but updates on the remote are far behind the commits that have been made by the developer.  The GM model itself if hung up on parameter estimation.</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2213,7 +2223,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Java/Groovy</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2228,39 +2238,29 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>2009 H1N1 Influenza (Swine Flu) fit to Washington State University Student Health Center data set</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Healthcare facility network outbreak simulator</t>
+          <t>H1N1 Pandemic Data Estimation</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Provides flexible framework for agent-based simulation of outbreaks among in-patients in a generic-but-realistic network of short/long-stay hospitals and nursing homes, as well as interventions to mitigate transmission and inter-facility spread. Scenarios(s) Modeled:  Initial invasion of new pathogen / strain and/or endemic pathogens. Intervention scenarios for patient-targeted efforts including surveillance and isolation (contact precautions), vaccination, and anti-microbial drug treatment.</t>
+          <t>Describes an SIR model parameter estimation with an improved fit using least squares estimation over maximum likelihood estimation. Parameter estimated: Transmission rate, recovery rate, R0, number of initial infectives</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2270,12 +2270,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen(s); we have applied the model to carbapenem-resistant Enterobacteriaceae, C. difficile, and MRSA.</t>
+          <t>N/A (basic SIR)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Effort was made to convert the model to publicly available software Repast (by Willy Ray) but was not completed.</t>
+          <t>N/A (LSE, MLE)</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2300,174 +2300,174 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Local network of hospitals and nursing homes that directly exchange patients, as well as generic “community” component to track discharged / readmitted patients after and between hospital stays.</t>
+          <t>2009 H1N1 Influenza (Swine Flu) fit to Washington State University Student Health Center data set</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
+          <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Healthcare facility network outbreak simulator</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Provides flexible framework for agent-based simulation of outbreaks among in-patients in a generic-but-realistic network of short/long-stay hospitals and nursing homes, as well as interventions to mitigate transmission and inter-facility spread. Scenarios(s) Modeled:  Initial invasion of new pathogen / strain and/or endemic pathogens. Intervention scenarios for patient-targeted efforts including surveillance and isolation (contact precautions), vaccination, and anti-microbial drug treatment.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Damon Toth</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Damon.Toth@hsc.utah.edu</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Any healthcare-associated pathogen(s); we have applied the model to carbapenem-resistant Enterobacteriaceae, C. difficile, and MRSA.</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Effort was made to convert the model to publicly available software Repast (by Willy Ray) but was not completed.</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Anylogic</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Local network of hospitals and nursing homes that directly exchange patients, as well as generic “community” component to track discharged / readmitted patients after and between hospital stays.</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>Healthcare transmission epidemiology estimation at equilibrium</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Estimate the extent of patient-to-patient transmission and other quantities using admission prevalence and cross-sectional point-prevalence data for carriage of organisms among healthcare facility in-patients. Parameter estimated: Patient-to-patient transmission rate, facility reproduction number, rate of progression to infection, intervention effects if applicable. Estimates derived via solving differential equations at equilibrium and facility reproduction number equations.</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Damon Toth</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Any healthcare-transmissible pathogen with appropriate data; we have applied our tools to carbapenem-resistant Enterobacteriaceae, C. difficile, and S. aureus.</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort. Creating an R package for facility reproduction number calculations has been discussed.</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Parameter estimation </t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
         <is>
           <t>Appropriate for application to data sets for patient carriage prevalence at admission and cross-sectional in-patient prevalence, when these quantities are stable over time. Contextual data for length of stay, invasive infection rates, carriage duration and intervention efforts add utility. Useful for understanding transmission risk and threshold effects in healthcare facilities, and for estimating intervention effectiveness.</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>o	Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557._x000D_
 o	Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Herpes Vaccine Model</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>An ODE-based 6-compartment SI model with asymptomatic carriers and vaccinated classes to forecast the number of infections prevented with imperfect vaccination and infections prevented per vaccine administered. Parameter estimated: Highly correlated parameters determined using LHS PRCC. Scenarios(s) Modeled: Prophylactic (pre-exposure) vaccines, Therapeutic (post-exposure) vaccines, Parameter(s) Estimated: Highly correlated parameters determined using LHS PRCC</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Elissa Schwartz</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>ejs@wsu.edu</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>HSV-2 (Herpes Simplex Virus)</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Matlab program for uncertainty and sensitivity analysis (Latin Hypercube Sampling and Partial Rank Correlation Coefficient analysis) in development and nearing completion. Old C/C++ code is being recoded in Matlab and R and should be ready soon (~April 2024).</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Matlab</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling &amp; Parameter estimation</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>Low prevalence populations (general pop), high-risk populations (high prevalence pops)</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
-        </is>
-      </c>
-    </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HIV End Stage Kidney Disease Epidemic Model</t>
+          <t>Herpes Vaccine Model</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>An ODE-based model to predict future disease prevalence given the impact of drug therapy levels and its mechanism of action (i.e., stopping progression to disease or reducing deaths). Parameter estimated:  Growth rate, death rate, drug efficacy to block disease progression. Scenarios(s) Modeled: Rebound in prevalence due to insufficient therapy (e.g., like in Paxlovid rebound).</t>
+          <t>An ODE-based 6-compartment SI model with asymptomatic carriers and vaccinated classes to forecast the number of infections prevented with imperfect vaccination and infections prevented per vaccine administered. Parameter estimated: Highly correlated parameters determined using LHS PRCC. Scenarios(s) Modeled: Prophylactic (pre-exposure) vaccines, Therapeutic (post-exposure) vaccines, Parameter(s) Estimated: Highly correlated parameters determined using LHS PRCC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2482,17 +2482,17 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>End stage kidney disease among HIV-infected population</t>
+          <t>HSV-2 (Herpes Simplex Virus)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Coded in Matlab, Berkeley Madonna, or Excel. Very easy to code up and use.</t>
+          <t>Matlab program for uncertainty and sensitivity analysis (Latin Hypercube Sampling and Partial Rank Correlation Coefficient analysis) in development and nearing completion. Old C/C++ code is being recoded in Matlab and R and should be ready soon (~April 2024).</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Coded in Matlab, Berkeley Madonna, or Excel.</t>
+          <t>Matlab</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2522,179 +2522,179 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Progression to the severe disease state, after infection. For parameter estimation: Fitting exponential growth curves to data, using Excel</t>
+          <t>Low prevalence populations (general pop), high-risk populations (high prevalence pops)</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
+          <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>HIV End Stage Kidney Disease Epidemic Model</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>An ODE-based model to predict future disease prevalence given the impact of drug therapy levels and its mechanism of action (i.e., stopping progression to disease or reducing deaths). Parameter estimated:  Growth rate, death rate, drug efficacy to block disease progression. Scenarios(s) Modeled: Rebound in prevalence due to insufficient therapy (e.g., like in Paxlovid rebound).</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>End stage kidney disease among HIV-infected population</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Coded in Matlab, Berkeley Madonna, or Excel. Very easy to code up and use.</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Coded in Matlab, Berkeley Madonna, or Excel.</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling &amp; Parameter estimation</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Progression to the severe disease state, after infection. For parameter estimation: Fitting exponential growth curves to data, using Excel</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>Household epidemiology estimation from antibody data</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>Simultaneously estimate household importation risk, household secondary attack rate, and associated variability / heterogeneities using point-prevalence data for antibody positivity among household members. Parameter estimated: Household importation probability, household secondary attack rate, sensitivity / specificity of data for indicating prior infection, variability (dispersion) in transmissibility,  and heterogeneities in those quantities over age and/or other identifiable characteristics of individuals and households. Estimates derived via maximum likelihood for final household outbreak size equations.</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>Damon Toth</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>Any household-transmissible pathogen with appropriate data; we have applied our tools to SARS-CoV-2.</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>Published</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Parameter estimation </t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
         <is>
           <t>Appropriate for application to data sets for prevalence of antibody positivity (e.g. via testing of serological samples) from members of randomly sampled households; useful for understanding transmission risk in close-contact indoor settings and mechanisms of epidemiological differences across demographic factors. Can also be applied to residents/staff of small nursing homes.</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097._x000D_
 2-Manuscript with age-structured model in preparation</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Household transmission simulator</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Simulate household importation and within-household transmission across a population of households, and intervention effects, e.g. vaccination. Scenarios(s) Modeled: Household importation and transmission with variability in transmissibility and heterogeneity across age groups and vaccination status.</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Damon Toth</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Any household-transmissible pathogen; tool has previously been used for SARS-CoV-2</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>R code for basic simulation is publicly available [https://github.com/damontoth/householdTransmission]. Extensions with age heterogeneity and vaccination are under development. Could be packaged for wider use.</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>A population of households in a given area; previously applied to a distribution of households representative of Utah. Can also be applied to residents / staff of small nursing homes.</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
-        </is>
-      </c>
-    </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Impact of school opening model on SARS-CoV-2 community incidence and mortality</t>
+          <t>Household transmission simulator</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The goal of this statistical analysis was to compare SARS-CoV-2 community incidence and mortality rates across schools that opened in in-person, remote, or hybrid mode. Measure(s) of Economic Impact: Infections and mortality</t>
+          <t>Simulate household importation and within-household transmission across a population of households, and intervention effects, e.g. vaccination. Scenarios(s) Modeled: Household importation and transmission with variability in transmissibility and heterogeneity across age groups and vaccination status.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2704,12 +2704,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Any household-transmissible pathogen; tool has previously been used for SARS-CoV-2</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>The Stata code for this analysis was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>R code for basic simulation is publicly available [https://github.com/damontoth/householdTransmission]. Extensions with age heterogeneity and vaccination are under development. Could be packaged for wider use.</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2734,39 +2734,39 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Statistical Model - Forecasting</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>The statistical model was developed using data on school mode from Burbio, SARS-CoV-2 and mortality rates from CDC, and mobility data from Google.</t>
+          <t>A population of households in a given area; previously applied to a distribution of households representative of Utah. Can also be applied to residents / staff of small nursing homes.</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>https://www.nature.com/articles/s41591-021-01563-8</t>
+          <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Inpatient antibiotic prescribing and effects simulator</t>
+          <t>Impact of school opening model on SARS-CoV-2 community incidence and mortality</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Simulate realistic rates and timing / duration / types of antibiotic administration to hospital inpatients and their effects on microbial transmission and infection, and antibiotic stewardship effects. Scenarios(s) Modeled:  Prescribing patterns of different types of antibiotics based on U.S. data; intervention scenarios for reducing prescribing, shortening duration of courses, and altering types of antibiotics used.</t>
+          <t>The goal of this statistical analysis was to compare SARS-CoV-2 community incidence and mortality rates across schools that opened in in-person, remote, or hybrid mode. Measure(s) of Economic Impact: Infections and mortality</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2776,12 +2776,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Any pathogen with supportable assumptions for antibiotic effects on hospital epidemiology; we have applied our tools to C. difficile.</t>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>R code is organized and documented but not publicly available. Could be made publicly available or packaged for use with moderate effort.</t>
+          <t>The Stata code for this analysis was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2806,29 +2806,29 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Statistical Model - Forecasting</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Single facility or small network of facilities</t>
+          <t>The statistical model was developed using data on school mode from Burbio, SARS-CoV-2 and mortality rates from CDC, and mobility data from Google.</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>https://www.nature.com/articles/s41591-021-01563-8</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Long-term acute care hospital (LTACH) intervention model</t>
+          <t>Inpatient antibiotic prescribing and effects simulator</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
+          <t>Simulate realistic rates and timing / duration / types of antibiotic administration to hospital inpatients and their effects on microbial transmission and infection, and antibiotic stewardship effects. Scenarios(s) Modeled:  Prescribing patterns of different types of antibiotics based on U.S. data; intervention scenarios for reducing prescribing, shortening duration of courses, and altering types of antibiotics used.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2848,12 +2848,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
+          <t>Any pathogen with supportable assumptions for antibiotic effects on hospital epidemiology; we have applied our tools to C. difficile.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>R code is organized and documented but not publicly available. Could be made publicly available or packaged for use with moderate effort.</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2883,49 +2883,49 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
+          <t>Single facility or small network of facilities</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Monolix</t>
+          <t>Long-term acute care hospital (LTACH) intervention model</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
+          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2935,12 +2935,12 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2950,39 +2950,39 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>https://monolix.lixoft.com/</t>
+          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Monolix</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2992,12 +2992,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Any hospital admission</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3007,12 +3007,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3022,59 +3022,54 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3084,7 +3079,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -3104,49 +3099,54 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3171,54 +3171,54 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,59 +3243,54 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3305,7 +3300,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3325,54 +3320,54 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3397,39 +3392,44 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3439,12 +3439,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3469,59 +3469,69 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3529,66 +3539,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3596,36 +3601,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -3635,12 +3640,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3650,7 +3655,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3665,39 +3670,34 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3742,24 +3742,24 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3779,12 +3779,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3814,34 +3814,34 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3851,12 +3851,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3881,54 +3881,54 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3953,54 +3953,54 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4025,39 +4025,39 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -4067,12 +4067,12 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4097,39 +4097,39 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4139,12 +4139,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -4169,64 +4169,69 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4241,69 +4246,59 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Vaccine Equity</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>An emerging infectious disease</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4318,82 +4313,159 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G57" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr">
+      <c r="M57" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N56" t="inlineStr">
+      <c r="N57" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Add linkeR to software packages
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2895,42 +2895,37 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Long-term acute care hospital (LTACH) intervention model</t>
+          <t>linkeR: Effortless Linked Views for Shiny Applications</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
+          <t>linkeR makes it effortless to create linked views in Shiny applications. When users interact with one component (like clicking a map marker), all related components (tables, charts, other maps) automatically update to show corresponding information.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Jake Wagoner</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>jakew@sci.utah.edu</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2940,64 +2935,64 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R Shiny Developers</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Moderate Programming</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
+          <t>Developer Tool</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
+          <t>https://epiforesite.github.io/linkeR/</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/linkeR/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Monolix</t>
+          <t>Long-term acute care hospital (LTACH) intervention model</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
+          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3007,12 +3002,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3022,39 +3017,39 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>https://monolix.lixoft.com/</t>
+          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Monolix</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3064,12 +3059,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Any hospital admission</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3079,12 +3074,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3094,59 +3089,54 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3156,7 +3146,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3176,49 +3166,54 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3228,7 +3223,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,54 +3238,54 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3300,7 +3295,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3315,59 +3310,54 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3377,7 +3367,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3397,54 +3387,54 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3469,39 +3459,44 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -3511,12 +3506,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3531,7 +3526,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3541,59 +3536,69 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3601,66 +3606,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3668,36 +3668,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3737,39 +3737,34 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3779,12 +3774,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3794,7 +3789,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3814,24 +3809,24 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3851,12 +3846,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3866,7 +3861,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3886,34 +3881,34 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3923,12 +3918,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3938,7 +3933,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3953,54 +3948,54 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4010,7 +4005,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -4025,54 +4020,54 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4097,39 +4092,39 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4139,12 +4134,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4174,34 +4169,34 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4211,12 +4206,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4226,7 +4221,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -4241,64 +4236,69 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4313,69 +4313,59 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Vaccine Equity</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>An emerging infectious disease</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4390,82 +4380,159 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G58" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr">
+      <c r="M58" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N57" t="inlineStr">
+      <c r="N58" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Add linkeR to software packages (#51)
* Add linkeR to software packages

* Automatic README update
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2895,42 +2895,37 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Long-term acute care hospital (LTACH) intervention model</t>
+          <t>linkeR: Effortless Linked Views for Shiny Applications</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
+          <t>linkeR makes it effortless to create linked views in Shiny applications. When users interact with one component (like clicking a map marker), all related components (tables, charts, other maps) automatically update to show corresponding information.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Jake Wagoner</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>jakew@sci.utah.edu</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2940,64 +2935,64 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R Shiny Developers</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Moderate Programming</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
+          <t>Developer Tool</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
+          <t>https://epiforesite.github.io/linkeR/</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/linkeR/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Monolix</t>
+          <t>Long-term acute care hospital (LTACH) intervention model</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
+          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3007,12 +3002,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3022,39 +3017,39 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>https://monolix.lixoft.com/</t>
+          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Monolix</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3064,12 +3059,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Any hospital admission</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3079,12 +3074,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3094,59 +3089,54 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3156,7 +3146,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3176,49 +3166,54 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3228,7 +3223,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,54 +3238,54 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3300,7 +3295,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3315,59 +3310,54 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3377,7 +3367,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3397,54 +3387,54 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3469,39 +3459,44 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -3511,12 +3506,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3531,7 +3526,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3541,59 +3536,69 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3601,66 +3606,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3668,36 +3668,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3707,12 +3707,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3737,39 +3737,34 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3779,12 +3774,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3794,7 +3789,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3814,24 +3809,24 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3851,12 +3846,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3866,7 +3861,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3886,34 +3881,34 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3923,12 +3918,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3938,7 +3933,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3953,54 +3948,54 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4010,7 +4005,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -4025,54 +4020,54 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4097,39 +4092,39 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4139,12 +4134,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4174,34 +4169,34 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4211,12 +4206,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4226,7 +4221,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -4241,64 +4236,69 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4313,69 +4313,59 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Vaccine Equity</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>An emerging infectious disease</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4390,82 +4380,159 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G58" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr">
+      <c r="M58" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N57" t="inlineStr">
+      <c r="N58" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
added rbranding and updated multigroup-vax, rendered readme.
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3106,22 +3106,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Multigroup Vaccine Model</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -3129,29 +3129,24 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Any hospital admission</t>
-        </is>
-      </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3166,54 +3161,54 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
+          <t>https://github.com/EpiForeSITE/multigroup-vaccine</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://github.com/EpiForeSITE/multigroup-vaccine</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3223,7 +3218,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,49 +3238,54 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3295,7 +3295,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3310,54 +3310,54 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3382,59 +3382,54 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3444,7 +3439,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3464,54 +3459,54 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3536,39 +3531,44 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -3578,12 +3578,12 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3608,59 +3608,69 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3668,66 +3678,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3735,36 +3740,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3774,12 +3779,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3789,7 +3794,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3804,39 +3809,34 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3846,12 +3846,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3881,64 +3881,59 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>rbranding</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>An R package that facilitates the creation of Shiny applications and quarto documents with support for site-specific branding and styling.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Willy Ray</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>william.ray@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Public health professionals, dashboard and report builders</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -3948,39 +3943,39 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Developer Tool</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>https://epiforesite.github.io/branding-package/</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/branding-package</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -3990,12 +3985,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4005,7 +4000,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -4020,54 +4015,54 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4077,7 +4072,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -4092,39 +4087,39 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4134,12 +4129,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4149,7 +4144,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -4169,49 +4164,49 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4236,39 +4231,39 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -4278,12 +4273,12 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -4293,7 +4288,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -4308,54 +4303,59 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -4365,7 +4365,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4375,44 +4375,39 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -4422,12 +4417,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>An emerging infectious disease</t>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -4437,7 +4432,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -4457,82 +4452,226 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>Multigroup Vaccine Model</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Damon Toth</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>damon.toth@hcs.utah.edu</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>On development</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>MIT</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Modelers</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Parameter inputs for simulating the model</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B60" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G60" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
+      <c r="M60" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N58" t="inlineStr">
+      <c r="N60" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Add rbranding, rename vax-ex (#54)
* change vax-ex to multigroup

* add rbranding

* added rbranding and updated multigroup-vax, rendered readme.

* Automatic project status update

* Automatic README update

* delete README.html, update .gitignore to ignore html files

* Automatic project status update

---------

Co-authored-by: WillyRay <11864373+WillyRay@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3106,22 +3106,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Multigroup Vaccine Model</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -3129,29 +3129,24 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Any hospital admission</t>
-        </is>
-      </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3166,54 +3161,54 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
+          <t>https://github.com/EpiForeSITE/multigroup-vaccine</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://github.com/EpiForeSITE/multigroup-vaccine</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3223,7 +3218,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,49 +3238,54 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3295,7 +3295,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3310,54 +3310,54 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3382,59 +3382,54 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3444,7 +3439,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3464,54 +3459,54 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3536,39 +3531,44 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -3578,12 +3578,12 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3608,59 +3608,69 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3668,66 +3678,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3735,36 +3740,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3774,12 +3779,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3789,7 +3794,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3804,39 +3809,34 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3846,12 +3846,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3881,64 +3881,59 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>rbranding</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>An R package that facilitates the creation of Shiny applications and quarto documents with support for site-specific branding and styling.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Willy Ray</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>william.ray@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Public health professionals, dashboard and report builders</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -3948,39 +3943,39 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Developer Tool</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>https://epiforesite.github.io/branding-package/</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/branding-package</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -3990,12 +3985,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4005,7 +4000,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -4020,54 +4015,54 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4077,7 +4072,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -4092,39 +4087,39 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4134,12 +4129,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4149,7 +4144,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -4169,49 +4164,49 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4236,39 +4231,39 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -4278,12 +4273,12 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -4293,7 +4288,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -4308,54 +4303,59 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -4365,7 +4365,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4375,44 +4375,39 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Parameter estimation </t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -4422,12 +4417,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>An emerging infectious disease</t>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -4437,7 +4432,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -4457,82 +4452,226 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>Multigroup Vaccine Model</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Damon Toth</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>damon.toth@hcs.utah.edu</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>On development</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>MIT</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Modelers</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Parameter inputs for simulating the model</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B60" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G60" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
+      <c r="M60" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N58" t="inlineStr">
+      <c r="N60" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Add epitraxr.yml and update README
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -785,7 +785,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>We’ve used Mortality Mapping (mMAP), an existing epidemiologic and statistical analysis approach by Lu et al. [1,2] to estimate the cumulative incidence of symptomatic COVID-19 in Veterans in the United States. mMAP is a time series deconvolution method which infers the true COVID-19 case counts from reported COVID-19 deaths. It uses symptom onset to death distribution, smoothed time series of reported COVID-19 deaths, and symptomatic case fatality rate (sCFR) to estimate the distribution of symptomatic COVID-19 cases. We focus on the adjusted version of the mMAP approach presented by Lu et al., which tries to account for the unreported COVID-19 deaths. While Lu uses excess influenza and pneumonia deaths to account for unreported COVID-19 deaths, we have extended their approach by using excess all-cause deaths. </t>
+          <t xml:space="preserve">We’ve used Mortality Mapping (mMAP), an existing epidemiologic and statistical analysis approach by Lu et al. [1,2] to estimate the cumulative incidence of symptomatic COVID-19 in Veterans in the United States. mMAP is a time series deconvolution method which infers the true COVID-19 case counts from reported COVID-19 deaths. It uses symptom onset to death distribution, smoothed time series of reported COVID-19 deaths, and symptomatic case fatality rate (sCFR) to estimate the distribution of symptomatic COVID-19 cases. We focus on the adjusted version of the mMAP approach presented by Lu et al., which tries to account for the unreported COVID-19 deaths. While Lu uses excess influenza and pneumonia deaths to account for unreported COVID-19 deaths, we have extended their approach by using excess all-cause deaths. </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
+          <t xml:space="preserve">Under the following existing papers from others: 1-https://www.medrxiv.org/content/10.1101/2020.04.18.20070821v3.full.pdf , 2-https://journals.plos.org/ploscompbiol/article?id=10.1371/journal.pcbi.1008994 </t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1848,22 +1848,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>epiworld: Fast Agent-Based Epi Models</t>
+          <t>epitraxr: Manipulate Epitrax Data And Generate Reports</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
+          <t>R package for manipulating Epitrax data and generating reports. This tool is designed to simplify the process of working with Epitrax data, making it easier for public health professionals to analyze and report on disease surveillance data. It generates internal and public reports in CSV, Excel, or PDF formats.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>George G. Vega Yon</t>
+          <t>Andrew Pulsipher</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>george.vegayon@utah.edu</t>
+          <t>a.pulsipher@utah.edu</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1883,59 +1883,59 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>R, C++, Python, Webessembly</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Public Health Professionals</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Beginner</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>Epitrax data</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworld, https://github.com/UofUEpiBio/epiworldR/, https://github.com/UofUEpiBio/epiworldpy, https://github.com/UofUEpiBio/epiworldRShiny</t>
+          <t>https://epiforesite.github.io/epitraxr/, https://github.com/EpiForeSITE/epitraxr</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworld</t>
+          <t>https://github.com/EpiForeSITE/epitraxr</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>epiworld-forecasts: Automatic Disease Forecasting with epiworldR</t>
+          <t>epiworld: Fast Agent-Based Epi Models</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>epiworld-forecasts uses epiworldR, GitHub Actions, and Docker to generate disease forecasts that update automatically. While we provide an example forecast of COVID-19 case counts in Utah, this tool is an open-source, template repository that can easily be adapted to generate forecasts for different diseases.</t>
+          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Andrew Pulsipher</t>
+          <t>George G. Vega Yon</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>a.pulsipher@utah.edu</t>
+          <t>george.vegayon@utah.edu</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1955,12 +1955,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>R, C++, Python, Webessembly</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Forecasters</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1970,44 +1970,44 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Automation pipeline tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Data sources, model definition, calibration steps</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/epiworld-forecasts, https://epiforesite.github.io/epiworld-forecasts/, https://github.com/UofUEpiBio/epiworldR/</t>
+          <t>https://github.com/UofUEpiBio/epiworld, https://github.com/UofUEpiBio/epiworldR/, https://github.com/UofUEpiBio/epiworldpy, https://github.com/UofUEpiBio/epiworldRShiny</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/epiworld-forecasts</t>
+          <t>https://github.com/UofUEpiBio/epiworld</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>epiworldpy: A python wrapper for epiworld</t>
+          <t>epiworld-forecasts: Automatic Disease Forecasting with epiworldR</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
+          <t>epiworld-forecasts uses epiworldR, GitHub Actions, and Docker to generate disease forecasts that update automatically. While we provide an example forecast of COVID-19 case counts in Utah, this tool is an open-source, template repository that can easily be adapted to generate forecasts for different diseases.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>George G. Vega Yon, Milo Banks</t>
+          <t>Andrew Pulsipher</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>george.vegayon@utah.edu</t>
+          <t>a.pulsipher@utah.edu</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Alpha/Beta phase: ready for inital user testing but requires additional development and testing</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2027,12 +2027,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Forecasters</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2042,44 +2042,44 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Automation pipeline tool</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>Data sources, model definition, calibration steps</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+          <t>https://github.com/EpiForeSITE/epiworld-forecasts, https://epiforesite.github.io/epiworld-forecasts/, https://github.com/UofUEpiBio/epiworldR/</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+          <t>https://github.com/EpiForeSITE/epiworld-forecasts</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Excess Death Estimation</t>
+          <t>epiworldpy: A python wrapper for epiworld</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>The aberration detection methods introduced by Farrington et al. and later Noufaily et al. have been implemented to obtain weekly all-cause mortality data.</t>
+          <t>A flexible framework for Agent-Based Models (ABM), the 'epiworldR' package provides methods for prototyping disease outbreaks and transmission models using a 'C++' backend, making it very fast. It supports multiple epidemiological models, including the Susceptible-Infected-Susceptible (SIS), Susceptible-Infected-Removed (SIR), Susceptible-Exposed-Infected-Removed (SEIR), and others, involving arbitrary mitigation policies and multiple-disease models. Users can specify infectiousness/susceptibility rates as a function of agents' features, providing great complexity for the model dynamics. Furthermore, 'epiworldR' is ideal for simulation studies featuring large populations.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Vanessa Stevens or Wathsala Widanagamaachchi</t>
+          <t>George G. Vega Yon, Milo Banks</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>vanessa.stevens@hsc.utah.edu; vanessa.stevens@va.gov or wathsala.widanagamaachchi@hsc.utah.edu</t>
+          <t>george.vegayon@utah.edu</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2087,29 +2087,24 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>None.  Kelly believes this was all cause mortality estimation.</t>
-        </is>
-      </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>We already have a version of this in operations</t>
+          <t>Alpha/Beta phase: ready for inital user testing but requires additional development and testing</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2119,39 +2114,44 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Statistical Model - Forecasting</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Data sources for this include both inpatient and outpatient mortality records. The ‘surveillance’ package in R was used to implement both the original Farrington method and the Flexible Farrington method by Noufaily et al. depending on the options specified. Control slots are used to specify which options are to be used. These options are customizable, but a strength of Farrington-based algorithms is that they are relatively robust across applications. Many of the options we have used are based on algorithm defaults. Additionally, ‘Nobbs’ nowcasting package in R was used to address delays in death reporting before applying Flexible Farrington.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Not currently published.</t>
+          <t>https://github.com/UofUEpiBio/epiworldpy</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>https://github.com/UofUEpiBio/epiworldpy</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GeoCovid</t>
+          <t>Excess Death Estimation</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Shiny App for visualizing mobility data and COVID-19 cases in Buenos Aires province during March to December 2020.</t>
+          <t>The aberration detection methods introduced by Farrington et al. and later Noufaily et al. have been implemented to obtain weekly all-cause mortality data.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Maria del Pilar Fernandez</t>
+          <t>Vanessa Stevens or Wathsala Widanagamaachchi</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>pilar.fernandez@wsu.edu</t>
+          <t>vanessa.stevens@hsc.utah.edu; vanessa.stevens@va.gov or wathsala.widanagamaachchi@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2159,9 +2159,19 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>None.  Kelly believes this was all cause mortality estimation.</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Under development</t>
+          <t>We already have a version of this in operations</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2169,36 +2179,51 @@
           <t>R</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Statistical Model - Forecasting</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Data sources for this include both inpatient and outpatient mortality records. The ‘surveillance’ package in R was used to implement both the original Farrington method and the Flexible Farrington method by Noufaily et al. depending on the options specified. Control slots are used to specify which options are to be used. These options are customizable, but a strength of Farrington-based algorithms is that they are relatively robust across applications. Many of the options we have used are based on algorithm defaults. Additionally, ‘Nobbs’ nowcasting package in R was used to address delays in death reporting before applying Flexible Farrington.</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app, https://github.com/Fernandez-Lab-WSU/geocovid_bsas, https://fernandez-lab-wsu.github.io/geocovid-slides/slides.html#/geocovidar</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
+          <t>Not currently published.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Granular Modeling Framework/ICU</t>
+          <t>GeoCovid</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Implement 2 ICUs that match the CVICU at the University of Utah and the ICU at the Salt Lake City VA.  Model all empirical data collected by the GM project:  HCW movement and touch data as collected by the proximity sensors, Patient flow from the EHR, and micro data as sampled by the GM micro team.  Scenarios(s) Modeled: Sustained endemic HAI levels driven by importation into a 15-25 bed ICU.  Contamination and transmission via HCW movement and contact behaviors.  The simulation includes contamination of multiple surfaces in several room zones, contamination of patient surfaces via shedding and HCW surfaces via touching.  Room cleaning, isolation, and targeted treatment of HAI.  HCW visits include assigned networks between health care workers and patients as well as ad hoc visits.</t>
+          <t>Shiny App for visualizing mobility data and COVID-19 cases in Buenos Aires province during March to December 2020.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Willy Ray</t>
+          <t>Maria del Pilar Fernandez</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>william.ray@hcs.utah.edu</t>
+          <t>pilar.fernandez@wsu.edu</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2206,76 +2231,61 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Only C.Diff currently implemented, but all organisms sampled in the GM project were targeted.</t>
-        </is>
-      </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>The framework is developed in Java/Groovy in the Repast Simphony toolset.  It is intended to be useable to quickly model fresh scenarios relatively quickly.  In practice, it is currently only useable by Willy.  Willy is able to use it to develop new models and features in existing models fairly quickly, but no-one else will be able to do that at this point.  The GM model and the underlying framework are hosted on github, but updates on the remote are far behind the commits that have been made by the developer.  The GM model itself if hung up on parameter estimation.</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Under development</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Java/Groovy</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app, https://github.com/Fernandez-Lab-WSU/geocovid_bsas, https://fernandez-lab-wsu.github.io/geocovid-slides/slides.html#/geocovidar</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/geocovid_app</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H1N1 Pandemic Data Estimation</t>
+          <t>Granular Modeling Framework/ICU</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Describes an SIR model parameter estimation with an improved fit using least squares estimation over maximum likelihood estimation. Parameter estimated: Transmission rate, recovery rate, R0, number of initial infectives</t>
+          <t>Implement 2 ICUs that match the CVICU at the University of Utah and the ICU at the Salt Lake City VA.  Model all empirical data collected by the GM project:  HCW movement and touch data as collected by the proximity sensors, Patient flow from the EHR, and micro data as sampled by the GM micro team.  Scenarios(s) Modeled: Sustained endemic HAI levels driven by importation into a 15-25 bed ICU.  Contamination and transmission via HCW movement and contact behaviors.  The simulation includes contamination of multiple surfaces in several room zones, contamination of patient surfaces via shedding and HCW surfaces via touching.  Room cleaning, isolation, and targeted treatment of HAI.  HCW visits include assigned networks between health care workers and patients as well as ad hoc visits.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Willy Ray</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>william.ray@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>N/A (basic SIR)</t>
+          <t>Only C.Diff currently implemented, but all organisms sampled in the GM project were targeted.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>N/A (LSE, MLE)</t>
+          <t>The framework is developed in Java/Groovy in the Repast Simphony toolset.  It is intended to be useable to quickly model fresh scenarios relatively quickly.  In practice, it is currently only useable by Willy.  Willy is able to use it to develop new models and features in existing models fairly quickly, but no-one else will be able to do that at this point.  The GM model and the underlying framework are hosted on github, but updates on the remote are far behind the commits that have been made by the developer.  The GM model itself if hung up on parameter estimation.</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2285,7 +2295,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Java/Groovy</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2300,39 +2310,29 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>2009 H1N1 Influenza (Swine Flu) fit to Washington State University Student Health Center data set</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Healthcare facility network outbreak simulator</t>
+          <t>H1N1 Pandemic Data Estimation</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Provides flexible framework for agent-based simulation of outbreaks among in-patients in a generic-but-realistic network of short/long-stay hospitals and nursing homes, as well as interventions to mitigate transmission and inter-facility spread. Scenarios(s) Modeled:  Initial invasion of new pathogen / strain and/or endemic pathogens. Intervention scenarios for patient-targeted efforts including surveillance and isolation (contact precautions), vaccination, and anti-microbial drug treatment.</t>
+          <t>Describes an SIR model parameter estimation with an improved fit using least squares estimation over maximum likelihood estimation. Parameter estimated: Transmission rate, recovery rate, R0, number of initial infectives</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2342,12 +2342,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen(s); we have applied the model to carbapenem-resistant Enterobacteriaceae, C. difficile, and MRSA.</t>
+          <t>N/A (basic SIR)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Effort was made to convert the model to publicly available software Repast (by Willy Ray) but was not completed.</t>
+          <t>N/A (LSE, MLE)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2372,174 +2372,174 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Local network of hospitals and nursing homes that directly exchange patients, as well as generic “community” component to track discharged / readmitted patients after and between hospital stays.</t>
+          <t>2009 H1N1 Influenza (Swine Flu) fit to Washington State University Student Health Center data set</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
+          <t>https://doi.org/10.1016/j.mbs.2015.03.007</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Healthcare facility network outbreak simulator</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Provides flexible framework for agent-based simulation of outbreaks among in-patients in a generic-but-realistic network of short/long-stay hospitals and nursing homes, as well as interventions to mitigate transmission and inter-facility spread. Scenarios(s) Modeled:  Initial invasion of new pathogen / strain and/or endemic pathogens. Intervention scenarios for patient-targeted efforts including surveillance and isolation (contact precautions), vaccination, and anti-microbial drug treatment.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Damon Toth</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Damon.Toth@hsc.utah.edu</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Any healthcare-associated pathogen(s); we have applied the model to carbapenem-resistant Enterobacteriaceae, C. difficile, and MRSA.</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Effort was made to convert the model to publicly available software Repast (by Willy Ray) but was not completed.</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Anylogic</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Local network of hospitals and nursing homes that directly exchange patients, as well as generic “community” component to track discharged / readmitted patients after and between hospital stays.</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>1-Slayton R, Toth D, Lee B, Tanner W, Bartsch S, Khader K, Wong K, Brown K, McKinnell J, Ray W, Miller L, Rubin M, Kim D, Adler F, Cao C, Avery L, Stone N, Kallen A, Samore M, Huang S, Fridkin S, Jernigan J (2015). Vital Signs: estimated effects of a coordinated approach for action to reduce antibiotic-resistant infections in health care facilities - United States. MMWR Morb Mortal Wkly Rep, 64(30), 826-831. https://doi.org/10.1111/ajt.13555. 2-Toth D, Khader K, Slayton R, Kallen A, Gundlapalli A, O'Hagan J, Fiore A, Rubin M, Jernigan J, Samore M (2017). The potential for interventions in a long-term acute care hospital to reduce transmission of carbapenem-resistant Enterobacteriaceae in affiliated healthcare facilities. Clin Infect Dis, 65(4), 581-587. https://doi.org/10.1093/cid/cix370., 3-Toth D, Keegan L, Samore M, Khader K, O'Hagan J, Yu H, Quintana A, Swerdlow D (2020). Modeling the potential impact of administering vaccines against Clostridioides difficile infection to individuals in healthcare facilities. Vaccine, 38(37), 5927-5932. https://doi.org/10.1016/j.vaccine.2020.06.081.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>Healthcare transmission epidemiology estimation at equilibrium</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>Estimate the extent of patient-to-patient transmission and other quantities using admission prevalence and cross-sectional point-prevalence data for carriage of organisms among healthcare facility in-patients. Parameter estimated: Patient-to-patient transmission rate, facility reproduction number, rate of progression to infection, intervention effects if applicable. Estimates derived via solving differential equations at equilibrium and facility reproduction number equations.</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Damon Toth</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>Any healthcare-transmissible pathogen with appropriate data; we have applied our tools to carbapenem-resistant Enterobacteriaceae, C. difficile, and S. aureus.</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort. Creating an R package for facility reproduction number calculations has been discussed.</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Parameter estimation </t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
         <is>
           <t>Appropriate for application to data sets for patient carriage prevalence at admission and cross-sectional in-patient prevalence, when these quantities are stable over time. Contextual data for length of stay, invasive infection rates, carriage duration and intervention efforts add utility. Useful for understanding transmission risk and threshold effects in healthcare facilities, and for estimating intervention effectiveness.</t>
         </is>
       </c>
-      <c r="N29" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>o	Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557._x000D_
 o	Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Herpes Vaccine Model</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>An ODE-based 6-compartment SI model with asymptomatic carriers and vaccinated classes to forecast the number of infections prevented with imperfect vaccination and infections prevented per vaccine administered. Parameter estimated: Highly correlated parameters determined using LHS PRCC. Scenarios(s) Modeled: Prophylactic (pre-exposure) vaccines, Therapeutic (post-exposure) vaccines, Parameter(s) Estimated: Highly correlated parameters determined using LHS PRCC</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Elissa Schwartz</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>ejs@wsu.edu</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>HSV-2 (Herpes Simplex Virus)</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Matlab program for uncertainty and sensitivity analysis (Latin Hypercube Sampling and Partial Rank Correlation Coefficient analysis) in development and nearing completion. Old C/C++ code is being recoded in Matlab and R and should be ready soon (~April 2024).</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Matlab</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling &amp; Parameter estimation</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Low prevalence populations (general pop), high-risk populations (high prevalence pops)</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
-        </is>
-      </c>
-    </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HIV End Stage Kidney Disease Epidemic Model</t>
+          <t>Herpes Vaccine Model</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>An ODE-based model to predict future disease prevalence given the impact of drug therapy levels and its mechanism of action (i.e., stopping progression to disease or reducing deaths). Parameter estimated:  Growth rate, death rate, drug efficacy to block disease progression. Scenarios(s) Modeled: Rebound in prevalence due to insufficient therapy (e.g., like in Paxlovid rebound).</t>
+          <t>An ODE-based 6-compartment SI model with asymptomatic carriers and vaccinated classes to forecast the number of infections prevented with imperfect vaccination and infections prevented per vaccine administered. Parameter estimated: Highly correlated parameters determined using LHS PRCC. Scenarios(s) Modeled: Prophylactic (pre-exposure) vaccines, Therapeutic (post-exposure) vaccines, Parameter(s) Estimated: Highly correlated parameters determined using LHS PRCC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>End stage kidney disease among HIV-infected population</t>
+          <t>HSV-2 (Herpes Simplex Virus)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Coded in Matlab, Berkeley Madonna, or Excel. Very easy to code up and use.</t>
+          <t>Matlab program for uncertainty and sensitivity analysis (Latin Hypercube Sampling and Partial Rank Correlation Coefficient analysis) in development and nearing completion. Old C/C++ code is being recoded in Matlab and R and should be ready soon (~April 2024).</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Coded in Matlab, Berkeley Madonna, or Excel.</t>
+          <t>Matlab</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2594,179 +2594,179 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Progression to the severe disease state, after infection. For parameter estimation: Fitting exponential growth curves to data, using Excel</t>
+          <t>Low prevalence populations (general pop), high-risk populations (high prevalence pops)</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
+          <t>1-https://doi.org/10.1086/429299  2-https://doi.org/10.4161/hv.4529</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>HIV End Stage Kidney Disease Epidemic Model</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>An ODE-based model to predict future disease prevalence given the impact of drug therapy levels and its mechanism of action (i.e., stopping progression to disease or reducing deaths). Parameter estimated:  Growth rate, death rate, drug efficacy to block disease progression. Scenarios(s) Modeled: Rebound in prevalence due to insufficient therapy (e.g., like in Paxlovid rebound).</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>End stage kidney disease among HIV-infected population</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Coded in Matlab, Berkeley Madonna, or Excel. Very easy to code up and use.</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Coded in Matlab, Berkeley Madonna, or Excel.</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling &amp; Parameter estimation</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Progression to the severe disease state, after infection. For parameter estimation: Fitting exponential growth curves to data, using Excel</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>1-https://journals.lww.com/jasn/fulltext/2005/08000/highly_active_antiretroviral_therapy_and_the.23.aspx 2- https://doi.org/10.5206/mase/10852   3-https://ir.library.illinoisstate.edu/spora/vol6/iss1/6/.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>Household epidemiology estimation from antibody data</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>Simultaneously estimate household importation risk, household secondary attack rate, and associated variability / heterogeneities using point-prevalence data for antibody positivity among household members. Parameter estimated: Household importation probability, household secondary attack rate, sensitivity / specificity of data for indicating prior infection, variability (dispersion) in transmissibility,  and heterogeneities in those quantities over age and/or other identifiable characteristics of individuals and households. Estimates derived via maximum likelihood for final household outbreak size equations.</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>Damon Toth</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Any household-transmissible pathogen with appropriate data; we have applied our tools to SARS-CoV-2.</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>Published</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Parameter estimation </t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
         <is>
           <t>Appropriate for application to data sets for prevalence of antibody positivity (e.g. via testing of serological samples) from members of randomly sampled households; useful for understanding transmission risk in close-contact indoor settings and mechanisms of epidemiological differences across demographic factors. Can also be applied to residents/staff of small nursing homes.</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr">
+      <c r="N33" t="inlineStr">
         <is>
           <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097._x000D_
 2-Manuscript with age-structured model in preparation</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Household transmission simulator</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Simulate household importation and within-household transmission across a population of households, and intervention effects, e.g. vaccination. Scenarios(s) Modeled: Household importation and transmission with variability in transmissibility and heterogeneity across age groups and vaccination status.</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Damon Toth</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Any household-transmissible pathogen; tool has previously been used for SARS-CoV-2</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>R code for basic simulation is publicly available [https://github.com/damontoth/householdTransmission]. Extensions with age heterogeneity and vaccination are under development. Could be packaged for wider use.</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>A population of households in a given area; previously applied to a distribution of households representative of Utah. Can also be applied to residents / staff of small nursing homes.</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
-        </is>
-      </c>
-    </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Impact of school opening model on SARS-CoV-2 community incidence and mortality</t>
+          <t>Household transmission simulator</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>The goal of this statistical analysis was to compare SARS-CoV-2 community incidence and mortality rates across schools that opened in in-person, remote, or hybrid mode. Measure(s) of Economic Impact: Infections and mortality</t>
+          <t>Simulate household importation and within-household transmission across a population of households, and intervention effects, e.g. vaccination. Scenarios(s) Modeled: Household importation and transmission with variability in transmissibility and heterogeneity across age groups and vaccination status.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2776,12 +2776,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Any household-transmissible pathogen; tool has previously been used for SARS-CoV-2</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>The Stata code for this analysis was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>R code for basic simulation is publicly available [https://github.com/damontoth/householdTransmission]. Extensions with age heterogeneity and vaccination are under development. Could be packaged for wider use.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2806,39 +2806,39 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Statistical Model - Forecasting</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>The statistical model was developed using data on school mode from Burbio, SARS-CoV-2 and mortality rates from CDC, and mobility data from Google.</t>
+          <t>A population of households in a given area; previously applied to a distribution of households representative of Utah. Can also be applied to residents / staff of small nursing homes.</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>https://www.nature.com/articles/s41591-021-01563-8</t>
+          <t>1-Toth D, Beams A, Keegan L, Zhang Y, Greene T, Orleans B, Seegert N, Looney A, Alder S, Samore M (2021). High variability in transmission of SARS-CoV-2 within households and implications for control. PLoS ONE 16(11): e0259097. https://doi.org/10.1371/journal.pone.0259097. 2-Manuscripts with age-structured model and vaccination model in preparation</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Inpatient antibiotic prescribing and effects simulator</t>
+          <t>Impact of school opening model on SARS-CoV-2 community incidence and mortality</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Simulate realistic rates and timing / duration / types of antibiotic administration to hospital inpatients and their effects on microbial transmission and infection, and antibiotic stewardship effects. Scenarios(s) Modeled:  Prescribing patterns of different types of antibiotics based on U.S. data; intervention scenarios for reducing prescribing, shortening duration of courses, and altering types of antibiotics used.</t>
+          <t>The goal of this statistical analysis was to compare SARS-CoV-2 community incidence and mortality rates across schools that opened in in-person, remote, or hybrid mode. Measure(s) of Economic Impact: Infections and mortality</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -2848,12 +2848,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Any pathogen with supportable assumptions for antibiotic effects on hospital epidemiology; we have applied our tools to C. difficile.</t>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>R code is organized and documented but not publicly available. Could be made publicly available or packaged for use with moderate effort.</t>
+          <t>The Stata code for this analysis was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -2878,29 +2878,29 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Statistical Model - Forecasting</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Single facility or small network of facilities</t>
+          <t>The statistical model was developed using data on school mode from Burbio, SARS-CoV-2 and mortality rates from CDC, and mobility data from Google.</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>https://www.nature.com/articles/s41591-021-01563-8</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Long-term acute care hospital (LTACH) intervention model</t>
+          <t>Inpatient antibiotic prescribing and effects simulator</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
+          <t>Simulate realistic rates and timing / duration / types of antibiotic administration to hospital inpatients and their effects on microbial transmission and infection, and antibiotic stewardship effects. Scenarios(s) Modeled:  Prescribing patterns of different types of antibiotics based on U.S. data; intervention scenarios for reducing prescribing, shortening duration of courses, and altering types of antibiotics used.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2920,12 +2920,12 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
+          <t>Any pathogen with supportable assumptions for antibiotic effects on hospital epidemiology; we have applied our tools to C. difficile.</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>R code is organized and documented but not publicly available. Could be made publicly available or packaged for use with moderate effort.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2955,49 +2955,49 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
+          <t>Single facility or small network of facilities</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Monolix</t>
+          <t>Long-term acute care hospital (LTACH) intervention model</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
+          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3007,12 +3007,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3022,39 +3022,39 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>https://monolix.lixoft.com/</t>
+          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Monolix</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3064,12 +3064,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Any hospital admission</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3079,12 +3079,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3094,59 +3094,54 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Any elective hospital admission</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3156,7 +3151,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3176,49 +3171,54 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3243,54 +3243,54 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3315,59 +3315,54 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3377,7 +3372,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3397,54 +3392,54 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3469,39 +3464,44 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -3511,12 +3511,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3541,59 +3541,69 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3601,66 +3611,61 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>NA</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3668,36 +3673,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Parameter estimation </t>
-        </is>
-      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3707,12 +3712,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Rabies in Dogs</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3722,7 +3727,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3737,39 +3742,34 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3779,12 +3779,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -3814,24 +3814,24 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3851,12 +3851,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -3886,34 +3886,34 @@
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3923,12 +3923,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3953,54 +3953,54 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Scale is flexible.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -4025,54 +4025,54 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4097,39 +4097,39 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4139,12 +4139,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4169,39 +4169,39 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Parameter estimation </t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4211,12 +4211,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -4241,64 +4241,69 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>University of Utah circuit breaker model</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>Local storage</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4313,69 +4318,59 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>University of Utah</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Vaccine Equity</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>An emerging infectious disease</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4390,82 +4385,159 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G58" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr">
+      <c r="M58" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N57" t="inlineStr">
+      <c r="N58" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>

<commit_message>
Rebuild README after resolving merge conflict
</commit_message>
<xml_diff>
--- a/data/software.xlsx
+++ b/data/software.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2967,42 +2967,37 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Long-term acute care hospital (LTACH) intervention model</t>
+          <t>linkeR: Effortless Linked Views for Shiny Applications</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
+          <t>linkeR makes it effortless to create linked views in Shiny applications. When users interact with one component (like clicking a map marker), all related components (tables, charts, other maps) automatically update to show corresponding information.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Jake Wagoner</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>jakew@sci.utah.edu</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -3012,64 +3007,64 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R Shiny Developers</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Moderate Programming</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
+          <t>Developer Tool</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
+          <t>https://epiforesite.github.io/linkeR/</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/linkeR/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Monolix</t>
+          <t>Long-term acute care hospital (LTACH) intervention model</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
+          <t>Provides analytic framework for investigating patient-focused interventions to prevent transmission in high-risk healthcare facilities and their direct and population-level health impacts and threshold effects. Scenarios(s) Modeled: Intervention scenarios for surveillance and isolation (contact precautions), decolonization drugs, infection treatment, horizontal transmission reduction, and length of stay reduction.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Any</t>
+          <t>Any pathogen posing risk of hospital transmission among in-patients; we have applied the model to carbapenem-resistant Enterobacteriaceae.</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3079,12 +3074,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3094,39 +3089,39 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Dataset</t>
+          <t>Single-facility model tailored to data from Chicago area LTACHs experiencing CRE outbreaks; could be re-tailored to other facility types</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>https://monolix.lixoft.com/</t>
+          <t>1-Toth D, Khader K, Beams A, Samore M (2019). Model-based Assessment of the Effect of Contact Precautions Applied to Surveillance-detected Carriers of Carbapenemase-producing Enterobacteriaceae in Long-term Acute Care Hospitals, Clinical Infectious Diseases 69(Supplement_3), S206–S213. https://doi.org/10.1093/cid/ciz557. 2-Toth D, Samore M, Nelson R (2021), Economic Evaluations of New Antibiotics: The High Potential Value of Reducing Healthcare Transmission Through Decolonization, Clinical Infectious Diseases 72(Supplement_1), S34–S41. https://doi.org/10.1093/cid/ciaa1590.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
+          <t>Monolix</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
+          <t>Parameter estimation in non-linear mixed effect models. Parameter estimated: Any.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -3136,12 +3131,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Any hospital admission</t>
+          <t>Any</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>Currently using to estimate strength of innate immune response, half-maximal effector cell proliferation threshold, effector cell amplification rate, cytotoxic T lymphocyte killing rate, time to production of virus by a newly infected cell</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3151,12 +3146,12 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Monolix can be used either via a graphical user interface (GUI) or a command-line interface (CLI) for powerful scripting. R package available</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Pharmacometricians of preclinical and clinical groups can rely on Monolix for population analysis and to model PK/PD and other complex biochemical and physiological processes.</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3166,74 +3161,64 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
+          <t>Dataset</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Preprint ready by June</t>
-        </is>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>https://github.com/madhobi/multitask_unit_and_days</t>
+          <t>https://monolix.lixoft.com/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Net financial impact of halting elective admissions</t>
+          <t>Multigroup Vaccine Model</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Richard Nelson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>richard.nelson@utah.edu</t>
+          <t>damon.toth@hcs.utah.edu</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Any elective hospital admission</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Stata</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3248,49 +3233,54 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
+          <t>Parameter inputs for simulating the model</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
+          <t>https://github.com/EpiForeSITE/multigroup-vaccine</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/multigroup-vaccine</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Nowcasting</t>
+          <t>Multitask Model to Forecast Patient's Next Unit and Remaining Length of Stay</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
+          <t>Length of Stay prediction and unit transfer prediction tool. Scenarios(s) Modeled: In this multi-task learning model, we train the model to predict:Task-1: patient's unit label in next time step. Task-2: patient's remaining length of stay.The model inputs get updated on a daily basis and generates prediction accordingly.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
+          <t>Any hospital admission</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
+          <t>Software page: https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3300,7 +3290,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3315,54 +3305,59 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Nowcasting tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
+          <t>This is the source code for building a deep learning model using multi-task learning (MTL) approach. The model is designed to train and validate on data prepared from Electronic Health Records (EHRs). The model was designed to learn and predict adaptively along the patient's stay. The model appends new data about the patient as it becomes available and update the prediction value accordingly.</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
+          <t>Preprint ready by June</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>https://github.com/madhobi/multitask_unit_and_days</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
+          <t>Net financial impact of halting elective admissions</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
+          <t>The goal of this model was to estimate the net financial impact to the hospital of halting elective admissions due to a COVID-19 surge. Measure(s) of Economic Impact: Hospital profit</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ananth Kalyanaraman</t>
+          <t>Richard Nelson</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ananth@wsu.edu</t>
+          <t>richard.nelson@utah.edu</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>View trajectory data</t>
+          <t>Any elective hospital admission</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
+          <t>The SAS code for this model was developed in 2020-2021 ultimately leading to a publication in 2021 but has not been touched since. So it would likely need to be updated.</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3372,7 +3367,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>PhenoMapper extension</t>
+          <t>Stata</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3392,39 +3387,34 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
+          <t>The simulation model was developed using inputs from national sources such as US Census, American Hospital Association Annual Survey, and National Inpatient Sample</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>https://github.com/tdavislab/PhenoMapper</t>
+          <t>https://pubmed.ncbi.nlm.nih.gov/33427797/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
+          <t>Nowcasting</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Analysis of time series data based on stochastic dynamical systems models</t>
+          <t>Given the time lag between laboratory testing for disease and eventual reporting, we’ve developed a model which consumes data from both community and VA to predict “now” how many positive tests for a disease (COVID-19 in this context) will eventually be reported as positive.  A VA HSR&amp;D abstract is available.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3434,12 +3424,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Currently this has only been applied to COVID-19, but a similar approach could be feasible for other diseases as well.</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
+          <t>Still early in its maturity.  We’ve had this running but have not yet started consuming this by analysts or stakeholders to assess value or accuracy.</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -3449,7 +3439,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3464,59 +3454,54 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Nowcasting tool</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>SIR type epi models, Markov processes (partially observed)</t>
+          <t>Currently VA data used for features includes admissions, COVID lab orders and their results.   Python-based regression “nowcasting” model of gradient boosted trees, implemented with XGBoost and scikit-learn</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>https://github.com/kingaa/pomp</t>
+          <t>An abstract of this was presented at VS HSR&amp;D meeting.  The text of the abstract is here: https://www.hsrd.research.va.gov/meetings/2023/abstract-display.cfm?AbsNum= (There is also a poster)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
+          <t>PhenoMapper: an interactive toolbox for the visual exploration of phenomics data</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
+          <t>TDA tool that can possibly help us to view some trajectory data. Scenarios(s) Modeled: We demonstrate the utility of this new tool on real-world plant (e.g., maize) phenomics datasets.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Ananth Kalyanaraman</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>ananth@wsu.edu</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>COVID-19</t>
+          <t>View trajectory data</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>  Software page: https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3526,7 +3511,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>PhenoMapper extension</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -3541,54 +3526,59 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+          <t>PhenoMapper is an extension of Mapper Interactive, which is a web-based framework for interactive analysis and visualization of high-dimensional point cloud data built upon the mapper algorithm.Our approach uses the mapper framework to perform a topological analysis of the data, and subsequently render visual representations with built-in data analysis and machine learning capabilities.</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
+          <t>https://dl.acm.org/doi/abs/10.1145/3459930.3469511</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>https://github.com/tdavislab/PhenoMapper</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Post-acute care model</t>
+          <t>POMP (Aaron King’s tool, U. of Michigan)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
+          <t>Analysis of time series data based on stochastic dynamical systems models</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Elissa Schwartz</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>ejs@wsu.edu</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>https://kingaa.github.io/pomp/vignettes/getting_started.html</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3603,7 +3593,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Healthcare practitioners</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3618,54 +3608,69 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
+          <t>SIR type epi models, Markov processes (partially observed)</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
+          <t>https://github.com/kingaa/pomp</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>quadkeyr</t>
+          <t>pomp R code for the estimation of unknown parameters in a two-population SEIR model from data collected in Whitman County, Washington</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
+          <t>Build a two-population SEIR model using the pomp coding framework in R and estimate the unknown parameters in this model using the PMCMC algorithm. Parameter estimated: Transmission parameters (transmission within each population and transmission across the two-populations), testing probability, and overdispersion parameter.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Florencia D'Andrea,  Pilar Fernandez</t>
+          <t>Erin Clancey</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>COVID-19</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>Fully developed and documented.</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3673,36 +3678,41 @@
           <t>TBD</t>
         </is>
       </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Parameter estimation </t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>This model was developed to model COVID-19 in Whitman County, Washington. This location has distinct university (WSU) and community populations where COVID was transmitted differently within each population with minimal cross-population transmission.</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
-        </is>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
+          <t>The manuscript is currently available as a preprint https://www.medrxiv.org/content/10.1101/2024.01.10.24301116v1.full.pdf and submitted to the journal Epidemics.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
+          <t>Post-acute care model</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
+          <t>A basic model to plan for the post-acute care needs following a hospital surge</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Lindsay Keegan</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Lindsay.Keegan@utah.edu</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3712,12 +3722,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>SARS-CoV-2</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Developed but not documented</t>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3732,7 +3742,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Healthcare practitioners</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3742,54 +3752,49 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Based on post-discharge needs of UHealth patients, takes the output from a scenario model (hospitalizations/ICU beds needed) and projects care needs</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>The R code is developed, but not documented.</t>
+          <t>https://www.medrxiv.org/content/10.1101/2020.06.12.20129551v1</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>https://github.com/mattrmaloney/covid-post-acute-care</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Rabies</t>
+          <t>quadkeyr</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
+          <t>An R package designed to create raster images from QuadKey-identified data (Microsoft Bing Maps Tile System), aiming to simplify the analysis of Facebook mobility data.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>Florencia D'Andrea,  Pilar Fernandez</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Rabies in Dogs</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Python code is available on GitHub</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>TBD</t>
+          <t>Published</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3799,7 +3804,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Modelers</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -3807,41 +3812,36 @@
           <t>TBD</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Stylized district in Kenya</t>
-        </is>
-      </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr, https://joss.theoj.org/papers/10.21105/joss.06500</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>https://github.com/Fernandez-Lab-WSU/quadkeyr</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Room contamination simulator</t>
+          <t>R code to implement an ODE model using the Tau Leaping algorithm</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
+          <t>This code offers flexible implementation of an ODE model using the Tau Leaping algorithm in R without the need for a package.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3851,12 +3851,12 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Documented R code has been shared for use internally but not publicly available.</t>
+          <t>Developed but not documented</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3881,39 +3881,34 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Single hospital room containing in-patient and hospital worker visits</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>The R code is developed, but not documented.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>School outbreak simulator</t>
+          <t>Rabies</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
+          <t>Stochastic representation of pulsed and continuous rabies eradication. Scenarios(s) Modeled: Pulsed vs. continuous rabies elimination programs. A number of parameters regarding dog survival, reproduction, etc. are also amenable to scenario modeling.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Damon Toth</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Damon.Toth@hsc.utah.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3923,12 +3918,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
+          <t>Rabies in Dogs</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
+          <t>Python code is available on GitHub</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3938,7 +3933,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Anylogic</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -3958,64 +3953,59 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Single school setting based on data from U.S. elementary school and middle school</t>
+          <t>Stylized district in Kenya</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Serfling</t>
+          <t>rbranding</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
+          <t>An R package that facilitates the creation of Shiny applications and quarto documents with support for site-specific branding and styling.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Eric Lofgren</t>
+          <t>Willy Ray</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Eric.Lofgren@wsu.edu</t>
+          <t>william.ray@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Developed for influenza, but in principle any seasonal disease.</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
+          <t>On development</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>MIT</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>JMP</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>Public health professionals, dashboard and report builders</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4025,54 +4015,54 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Scale is flexible.</t>
+          <t>Developer Tool</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
+          <t>https://epiforesite.github.io/branding-package/</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/branding-package</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Statistical Alerts (time series)</t>
+          <t>Room contamination simulator</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
+          <t>Simulate dynamic levels of contamination in hospital room surfaces and on patients / healthcare workers in the room. Scenarios(s) Modeled: Shedding in-patient in hospital room, susceptible patient in contaminated room, healthcare worker performing patient care, room cleaning and hand hygiene interventions, use of personal protective equipment.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Kelly Peterson</t>
+          <t>Damon Toth</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
+          <t>Any healthcare-associated pathogen; we have applied the tool to C. difficile.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
+          <t>Documented R code has been shared for use internally but not publicly available.</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -4097,29 +4087,29 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Decision Support tool</t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
+          <t>Single hospital room containing in-patient and hospital worker visits</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Transmission estimation for outbreak clusters</t>
+          <t>School outbreak simulator</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
+          <t>Agent-based simulation of person-to-person transmission at schools over data-based dynamic proximity contact networks. Scenarios(s) Modeled:  Transmission modeled during school hours; can model interventions affecting the contact network and school attendance behavior.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -4139,12 +4129,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
+          <t>Influenza; could be repurposed for similarly transmitted diseases.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
+          <t>Written in Anylogic, a Java-based simulation software that is not free or publicly available. Code must be run on old machines that still have the software. Contact data are publicly available* and could be used as basis for simulation on other platforms. *https://royalsocietypublishing.org/doi/suppl/10.1098/rsif.2015.0279</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4154,7 +4144,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>Anylogic</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -4169,39 +4159,39 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Parameter estimation </t>
+          <t>Epidemic Model - Scenario Modeling</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
+          <t>Single school setting based on data from U.S. elementary school and middle school</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
+          <t>Toth D, Leecaster M, Pettey W, Gundlapalli A, Gao H, Rainey J, Uzicanin A, Samore M (2015). The role of heterogeneity in contact timing and duration in network models of influenza spread in schools. J R Soc Interface, 12(108), 20150279. https://doi.org/10.1098/rsif.2015.0279.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
+          <t>Serfling</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
+          <t>Classic Serfling-type regression model for seasonal diseases. Can be used to estimate both excess risk (based on breaching a threshold), or estimate the peak week and other parameters of a yearly epidemic curve.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Erin Clancey</t>
+          <t>Eric Lofgren</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>erin.clancey@wsu.edu</t>
+          <t>Eric.Lofgren@wsu.edu</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4211,12 +4201,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Uses measles as an example but is not specific to a target disease.</t>
+          <t>Developed for influenza, but in principle any seasonal disease.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Fully developed and documented.</t>
+          <t>Old code written in JMP, but should be easy to recode in R if the motivation is there.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -4226,7 +4216,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>JMP</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -4246,49 +4236,49 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Scale is flexible.</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>This tutorial is not designed to be published.</t>
+          <t>https://link.springer.com/chapter/10.1007/978-3-540-72608-1_11</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>University of Utah circuit breaker model</t>
+          <t>Statistical Alerts (time series)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+          <t>We have supported an Operations system for processing time series for “aberrations” (aka, “alerts”, “potential outbreaks”) for 8+ years in VA BASIC.  During this time, we’ve integrated several among the suite of algorithms available in the R package titled “surveillance”.  This includes several classes of numerical methods, of which some are window-based, control chart-based or trained linear models.  A brief presentation on this is attached here.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Lindsay Keegan</t>
+          <t>Kelly Peterson</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Lindsay.Keegan@utah.edu</t>
+          <t>kelly.peterson2@va.gov ;kelly.peterson@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>SARS-CoV-2</t>
+          <t>Many.  We use this system for hundreds of different case definitions, ranging from COVID-19 to Zika, to drug resistant organisms, to Dengue, etc.</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Local storage</t>
+          <t>This has been deployed for Operations for years, but each algorithm has different properties and parameters.  Kelly would say that our current parameters are better tuned but still not ideal.  A collection of curated time series and human identified “aberration events” would likely be helpful.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -4298,7 +4288,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -4313,29 +4303,29 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t>Decision Support tool</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>University of Utah</t>
+          <t>Currently this is VA time series, could be applied to any time series with some de-coupling.  As far as technology, currently we’ve implemented an implementation which is a Python wrapper (epysurv) over the R package mentioned above.  This was selected since the API is more consistent in that it attempts to match the popular scikit-learn package.  Further, BASIC has more experience in Python than R.</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>The way that we implement this system has not been published, but there are links for “surveillance” (https://cran.r-project.org/web/packages/surveillance/index.html)and “epysurv” packages (https://epysurv.readthedocs.io/en/latest/).</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Vaccine Equity</t>
+          <t>Transmission estimation for outbreak clusters</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+          <t>Provides estimates for individual-level transmission distribution (mean and variance) based on data from prior isolated outbreak clusters. Useful for quantifying the risk of superspreading events and the risk that future outbreaks will exceed a given threshold.Parameter estimated: Basic reproduction number; dispersion parameter quantifying variance in transmission; extensions estimate changes in reproduction number by generation, e.g. post-control reproduction number. Estimated via maximum likelihood using final size distribution equations for branching process models.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -4345,22 +4335,27 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>damon.toth@hcs.utah.edu</t>
+          <t>Damon.Toth@hsc.utah.edu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Applied to pathogens with subcritical transmission (R &lt; 1) though also relevant for emerging R &gt; 1 pathogens that have not (yet) produced widespread sustained transmission in the given context. We have applied the tool to Ebola and Middle East respiratory syndrome (MERS).</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>On development</t>
+          <t>R code used for publication results is reasonably organized and documented but not publicly available. Key functions have been shared and used by others; could be made publicly available or packaged for use with reasonable effort.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -4370,7 +4365,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Modelers</t>
+          <t>TBD</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4380,44 +4375,39 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Parameter inputs for simulating the model</t>
+          <t>Appropriate for pathogens that have produced a series of isolated, extinguished outbreak clusters following an initial introduction, e.g. zoonotic spillover events or infected incoming travelers followed by a chain of human-to-human transmissions.</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+          <t>1-Toth D, Gundlapalli A, Khader K, Pettey W, Rubin M, Adler F, Samore M (2015). Estimates of outbreak risk from new introductions of Ebola with immediate and delayed transmission control. Emerg Infect Dis, 21(8), 1402-1408. https://doi.org/10.3201/eid2108.150170. 2-Toth D, Tanner W, Khader K, Gundlapalli A (2016). Estimates of the risk of large or long-lasting outbreaks of Middle East respiratory syndrome after importations outside the Arabian Peninsula. Epidemics, 16, 27-32. https://doi.org/10.1016/j.epidem.2016.04.002.</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Vaccine Hesitancy Model</t>
+          <t>Two-part pomp tutorial to estimate parameters from an SIR model using PMCMC</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+          <t>To goal of this two-part tutorial is to demonstrate how to implement an SIR epidemiological model in the pomp R package in part 1, and then estimate the unknown parameters in part 2. The tutorial is designed to focus on the R code. Parameter estimated: This tutorial gives a specific example of estimating the transmission and testing probability parameters using pomp.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Elissa Schwartz</t>
+          <t>Erin Clancey</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ejs@wsu.edu</t>
+          <t>erin.clancey@wsu.edu</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -4427,12 +4417,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>An emerging infectious disease</t>
+          <t>Uses measles as an example but is not specific to a target disease.</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+          <t>Fully developed and documented.</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -4442,7 +4432,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Matlab, R, and Mathematica.</t>
+          <t>R</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -4457,87 +4447,303 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Epidemic Model - Scenario Modeling</t>
+          <t xml:space="preserve">Parameter estimation </t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Any population. Population size does not need to be constant.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+          <t>This tutorial is not designed to be published.</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>University of Utah circuit breaker model</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>A basic model of school closure for the University of Utah fall reopening. Scenarios(s) Modeled: Delay start, circuit breaker, end early.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Lindsay Keegan</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Lindsay.Keegan@utah.edu</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Local storage</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>University of Utah</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Multigroup Vaccine Model</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>A tool for exploring the effects of varying rates of vaccination among disparate socio-economic groups</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Damon Toth</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>damon.toth@hcs.utah.edu</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>On development</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>MIT</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Modelers</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Parameter inputs for simulating the model</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>https://github.com/EpiForeSITE/vaccine-equity-model</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Vaccine Hesitancy Model</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>An ODE (ordinary differential equation)-based SVEIR model with 3 compartments for symptoms (mild, moderate, severe) that can quantify the tradeoffs between vaccine efficacy and vaccine hesitancy on reducing the disease burden. Scenarios(s) Modeled: R0, cumulative infections, and deaths due to varying values of transmission rate, vaccine coverage rate, vaccine efficacy, and vaccine hesitancy. The vaccine efficacy required to compensate for different levels of vaccine hesitancy.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Elissa Schwartz</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>ejs@wsu.edu</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>An emerging infectious disease</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>On a computer in my research group. Coded in Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Matlab, R, and Mathematica.</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Epidemic Model - Scenario Modeling</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Any population. Population size does not need to be constant.</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17513758.2023.2298988</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
           <t>Vector Autoregression</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B61" t="inlineStr">
         <is>
           <t>To develop a forecasting model to predict the weekly abx use and abx resistant rate in VA</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>Yue Zhang</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>zhang.yue@hsc.utah.edu</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>AMR, abx use</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G61" t="inlineStr">
         <is>
           <t>Research or Development phase</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
         <is>
           <t>Statistical Model - Forecasting</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
+      <c r="M61" t="inlineStr">
         <is>
           <t>The objective of this study is to use multiple time series data to predict weekly abx use and resistant rates across multipe pathogens in the inpatient setting. Timeframe: 02/2007-03/2020</t>
         </is>
       </c>
-      <c r="N58" t="inlineStr">
+      <c r="N61" t="inlineStr">
         <is>
           <t>Not published but will</t>
         </is>

</xml_diff>